<commit_message>
improved (removed redundant tab?)
</commit_message>
<xml_diff>
--- a/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
+++ b/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\idiom_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{422F07CD-6BAF-471E-BCDE-988839958F61}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB0C15A8-C254-436B-8EDF-DECF20AA35F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3960" yWindow="2835" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="idiom_database" sheetId="1" r:id="rId1"/>
@@ -3938,14 +3938,14 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00B050"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4279,7 +4279,7 @@
   <dimension ref="A1:U255"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T17" sqref="T17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
moved some wrongly placed idioms
</commit_message>
<xml_diff>
--- a/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
+++ b/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\idiom_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF7C8167-327C-46E1-BF2D-C7F6CAD05212}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07481172-A30E-403D-B5AD-568C5A1FBE83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17325" yWindow="2250" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="idiom_database" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1477" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="1182">
   <si>
     <t>Idiom</t>
   </si>
@@ -2937,18 +2937,12 @@
     <t>[ lemma= "bord" ] [ lemma= "voor" ] [ pos_head = "lid" | pos_head = "vnw" ] [ pos_head = "adj" ]? [ lemma= "kop" ]</t>
   </si>
   <si>
-    <t>[ lemma= "gat" ] [ lemma= "in" ] [pos_head = "lid" | pos_head = "vnw"] [ pos_head = "adj" ]? [ lemma= "hoofd" ]</t>
-  </si>
-  <si>
     <t>[ lemma= "gat" ] [ lemma= "in" ] [ pos_head = "lid" | pos_head = "vnw" ] [ pos_head = "adj" ]? [ lemma= "hand" ]</t>
   </si>
   <si>
     <t>[ lemma= "stok" ] [ lemma= "achter" ] [ pos_head="lid" ] [ pos_head = "adj" ]? [ lemma= "deur" ]</t>
   </si>
   <si>
-    <t>[ lemma= "stuk" ] [ lemma= "in" ] [ pos_head="lid" ] [ pos_head = "adj" ]? [ lemma= "kraag" ]</t>
-  </si>
-  <si>
     <t>[ lemma= "vinger" ] [ lemma= "in" ] [ pos_head="lid" ] [ pos_head = "adj" ]? [ lemma= "pap" ]</t>
   </si>
   <si>
@@ -3574,6 +3568,15 @@
   </si>
   <si>
     <t>zoek op vertrouwen zonder letterlijke woordgrenzen</t>
+  </si>
+  <si>
+    <t>[ word = "gaatje" ] [ lemma= "in" ] [pos_head = "lid" | pos_head = "vnw"] [ pos_head = "adj" ]? [ lemma= "hoofd" ]</t>
+  </si>
+  <si>
+    <t>[ lemma= "stuk" ] [ lemma= "in" ] [ pos_head="lid" | pos_head = "vnw"] [ pos_head = "adj" ]? [ lemma= "kraag" ]</t>
+  </si>
+  <si>
+    <t>maken</t>
   </si>
 </sst>
 </file>
@@ -4472,8 +4475,8 @@
   </sheetPr>
   <dimension ref="A1:V237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S174" sqref="S174"/>
+    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A139" sqref="A139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4547,19 +4550,19 @@
         <v>723</v>
       </c>
       <c r="P1" t="s">
-        <v>1157</v>
+        <v>1155</v>
       </c>
       <c r="Q1" t="s">
-        <v>1156</v>
+        <v>1154</v>
       </c>
       <c r="R1" t="s">
-        <v>1060</v>
+        <v>1058</v>
       </c>
       <c r="S1" t="s">
         <v>946</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>1065</v>
+        <v>1063</v>
       </c>
       <c r="V1" t="s">
         <v>945</v>
@@ -4623,7 +4626,7 @@
         <v>1</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1070</v>
+        <v>1068</v>
       </c>
       <c r="T2" s="8"/>
     </row>
@@ -4871,7 +4874,7 @@
         <v>5</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>1068</v>
+        <v>1066</v>
       </c>
       <c r="T6" s="8"/>
     </row>
@@ -4933,7 +4936,7 @@
         <v>6</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>1069</v>
+        <v>1067</v>
       </c>
       <c r="T7" s="8"/>
     </row>
@@ -5492,7 +5495,7 @@
       </c>
       <c r="T16" s="8"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>422</v>
       </c>
@@ -5554,7 +5557,7 @@
       </c>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>122</v>
       </c>
@@ -5616,7 +5619,7 @@
       </c>
       <c r="T18" s="8"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>546</v>
       </c>
@@ -5678,7 +5681,7 @@
       </c>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>143</v>
       </c>
@@ -5740,7 +5743,7 @@
       </c>
       <c r="T20" s="8"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>239</v>
       </c>
@@ -5802,7 +5805,7 @@
       </c>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>88</v>
       </c>
@@ -5860,11 +5863,11 @@
         <v>21</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>1072</v>
+        <v>1070</v>
       </c>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>379</v>
       </c>
@@ -5926,7 +5929,7 @@
       </c>
       <c r="T23" s="8"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -5984,11 +5987,11 @@
         <v>23</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>1071</v>
+        <v>1069</v>
       </c>
       <c r="T24" s="8"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>512</v>
       </c>
@@ -6050,7 +6053,7 @@
       </c>
       <c r="T25" s="8"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>368</v>
       </c>
@@ -6112,7 +6115,7 @@
       </c>
       <c r="T26" s="8"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>364</v>
       </c>
@@ -6174,7 +6177,7 @@
       </c>
       <c r="T27" s="8"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>205</v>
       </c>
@@ -6236,7 +6239,7 @@
       </c>
       <c r="T28" s="8"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>623</v>
       </c>
@@ -6294,11 +6297,11 @@
         <v>28</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="T29" s="8"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>261</v>
       </c>
@@ -6360,7 +6363,7 @@
       </c>
       <c r="T30" s="8"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>41</v>
       </c>
@@ -6422,7 +6425,7 @@
       </c>
       <c r="T31" s="8"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>418</v>
       </c>
@@ -6480,9 +6483,12 @@
         <v>31</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>968</v>
+        <v>1179</v>
       </c>
       <c r="T32" s="8"/>
+      <c r="U32" t="s">
+        <v>1092</v>
+      </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
@@ -6542,7 +6548,7 @@
         <v>32</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="T33" s="8"/>
     </row>
@@ -6604,7 +6610,7 @@
         <v>33</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="T34" s="8"/>
     </row>
@@ -6666,7 +6672,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>971</v>
+        <v>1180</v>
       </c>
       <c r="T35" s="8"/>
     </row>
@@ -6728,7 +6734,7 @@
         <v>35</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="T36" s="8"/>
     </row>
@@ -6790,7 +6796,7 @@
         <v>36</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="T37" s="8"/>
     </row>
@@ -6914,7 +6920,7 @@
         <v>38</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="T39" s="8"/>
     </row>
@@ -6976,7 +6982,7 @@
         <v>39</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="T40" s="8"/>
     </row>
@@ -7038,7 +7044,7 @@
         <v>40</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>1073</v>
+        <v>1071</v>
       </c>
       <c r="T41" s="8"/>
     </row>
@@ -7162,7 +7168,7 @@
         <v>42</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="T43" s="8"/>
     </row>
@@ -7286,7 +7292,7 @@
         <v>44</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="T45" s="8"/>
     </row>
@@ -7348,7 +7354,7 @@
         <v>45</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="T46" s="8"/>
     </row>
@@ -7534,7 +7540,7 @@
         <v>48</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="T49" s="8"/>
     </row>
@@ -7596,7 +7602,7 @@
         <v>49</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="T50" s="8"/>
     </row>
@@ -7658,7 +7664,7 @@
         <v>50</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="T51" s="8"/>
     </row>
@@ -7720,7 +7726,7 @@
         <v>51</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="T52" s="8"/>
     </row>
@@ -7844,7 +7850,7 @@
         <v>53</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="T54" s="8"/>
     </row>
@@ -7906,7 +7912,7 @@
         <v>54</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="T55" s="8"/>
     </row>
@@ -7968,7 +7974,7 @@
         <v>55</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="T56" s="8"/>
     </row>
@@ -8030,7 +8036,7 @@
         <v>56</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="T57" s="8"/>
     </row>
@@ -8092,7 +8098,7 @@
         <v>57</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>1076</v>
+        <v>1074</v>
       </c>
       <c r="T58" s="8"/>
     </row>
@@ -8154,7 +8160,7 @@
         <v>58</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="T59" s="8"/>
     </row>
@@ -8216,7 +8222,7 @@
         <v>59</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="T60" s="8"/>
     </row>
@@ -8278,7 +8284,7 @@
         <v>60</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="T61" s="8"/>
     </row>
@@ -8340,7 +8346,7 @@
         <v>61</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>1077</v>
+        <v>1075</v>
       </c>
       <c r="T62" s="8"/>
     </row>
@@ -8402,7 +8408,7 @@
         <v>62</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="T63" s="8"/>
     </row>
@@ -8464,7 +8470,7 @@
         <v>63</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="T64" s="8"/>
     </row>
@@ -8526,7 +8532,7 @@
         <v>64</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="T65" s="8"/>
     </row>
@@ -8588,7 +8594,7 @@
         <v>65</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="T66" s="8"/>
     </row>
@@ -8650,7 +8656,7 @@
         <v>66</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="T67" s="8"/>
     </row>
@@ -8712,7 +8718,7 @@
         <v>67</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="T68" s="8"/>
     </row>
@@ -8774,7 +8780,7 @@
         <v>68</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="T69" s="8"/>
     </row>
@@ -8836,7 +8842,7 @@
         <v>69</v>
       </c>
       <c r="S70" s="3" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="T70" s="8"/>
     </row>
@@ -8898,7 +8904,7 @@
         <v>70</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="T71" s="8"/>
     </row>
@@ -9022,7 +9028,7 @@
         <v>72</v>
       </c>
       <c r="S73" s="3" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="T73" s="8"/>
     </row>
@@ -9084,7 +9090,7 @@
         <v>73</v>
       </c>
       <c r="S74" s="3" t="s">
-        <v>1078</v>
+        <v>1076</v>
       </c>
       <c r="T74" s="8"/>
     </row>
@@ -9146,7 +9152,7 @@
         <v>74</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>1079</v>
+        <v>1077</v>
       </c>
       <c r="T75" s="8"/>
     </row>
@@ -9208,7 +9214,7 @@
         <v>75</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>1080</v>
+        <v>1078</v>
       </c>
       <c r="T76" s="8"/>
     </row>
@@ -9270,7 +9276,7 @@
         <v>76</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="T77" s="8"/>
     </row>
@@ -9332,7 +9338,7 @@
         <v>77</v>
       </c>
       <c r="S78" s="3" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="T78" s="8"/>
     </row>
@@ -9394,7 +9400,7 @@
         <v>78</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="T79" s="8"/>
     </row>
@@ -9456,7 +9462,7 @@
         <v>79</v>
       </c>
       <c r="S80" s="3" t="s">
-        <v>1083</v>
+        <v>1081</v>
       </c>
       <c r="T80" s="8"/>
     </row>
@@ -9518,69 +9524,69 @@
         <v>80</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="T81" s="8"/>
     </row>
     <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>651</v>
+        <v>393</v>
       </c>
       <c r="B82">
-        <v>175</v>
+        <v>104</v>
       </c>
       <c r="C82" t="s">
-        <v>398</v>
+        <v>15</v>
       </c>
       <c r="D82">
-        <v>1020</v>
+        <v>239</v>
       </c>
       <c r="E82" s="1">
-        <v>6928</v>
-      </c>
-      <c r="F82" t="s">
-        <v>179</v>
+        <v>5479</v>
+      </c>
+      <c r="F82">
+        <v>2</v>
       </c>
       <c r="G82">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H82">
         <v>16</v>
       </c>
       <c r="I82">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="J82">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="K82" s="1">
-        <v>3147</v>
-      </c>
-      <c r="L82" s="1">
-        <v>1477</v>
+        <v>2081</v>
+      </c>
+      <c r="L82" t="s">
+        <v>394</v>
       </c>
       <c r="M82" t="s">
-        <v>652</v>
+        <v>395</v>
       </c>
       <c r="N82" t="s">
-        <v>653</v>
+        <v>396</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>886</v>
+        <v>917</v>
       </c>
       <c r="P82" t="str">
-        <f t="shared" si="8"/>
+        <f>IF(COUNTIF(S82,"*adj*")&gt;0,"+","-")</f>
         <v>+</v>
       </c>
       <c r="Q82" t="str">
-        <f t="shared" si="9"/>
-        <v>-</v>
+        <f>IF(COUNTIF(S82,"*word=*")&gt;0,"-","+")</f>
+        <v>+</v>
       </c>
       <c r="R82">
         <v>81</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>1084</v>
+        <v>1047</v>
       </c>
       <c r="T82" s="8"/>
     </row>
@@ -9642,7 +9648,7 @@
         <v>82</v>
       </c>
       <c r="S83" s="3" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="T83" s="8"/>
     </row>
@@ -9704,7 +9710,7 @@
         <v>83</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="T84" s="8"/>
     </row>
@@ -9766,7 +9772,7 @@
         <v>84</v>
       </c>
       <c r="S85" s="3" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="T85" s="8"/>
     </row>
@@ -9828,7 +9834,7 @@
         <v>85</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="T86" s="8"/>
     </row>
@@ -9890,7 +9896,7 @@
         <v>86</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="T87" s="8"/>
     </row>
@@ -9952,7 +9958,7 @@
         <v>87</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="T88" s="8"/>
     </row>
@@ -10014,7 +10020,7 @@
         <v>88</v>
       </c>
       <c r="S89" s="3" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="T89" s="8"/>
     </row>
@@ -10076,7 +10082,7 @@
         <v>89</v>
       </c>
       <c r="S90" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="T90" s="8"/>
     </row>
@@ -10138,7 +10144,7 @@
         <v>90</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="T91" s="8"/>
     </row>
@@ -10200,7 +10206,7 @@
         <v>91</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="T92" s="8"/>
     </row>
@@ -10262,7 +10268,7 @@
         <v>92</v>
       </c>
       <c r="S93" s="3" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="T93" s="8"/>
     </row>
@@ -10324,7 +10330,7 @@
         <v>93</v>
       </c>
       <c r="S94" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="T94" s="8"/>
     </row>
@@ -10386,7 +10392,7 @@
         <v>94</v>
       </c>
       <c r="S95" s="3" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="T95" s="8"/>
     </row>
@@ -10448,7 +10454,7 @@
         <v>95</v>
       </c>
       <c r="S96" s="3" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="T96" s="8"/>
     </row>
@@ -10510,7 +10516,7 @@
         <v>96</v>
       </c>
       <c r="S97" s="3" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="T97" s="8"/>
     </row>
@@ -10572,7 +10578,7 @@
         <v>97</v>
       </c>
       <c r="S98" s="3" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="T98" s="8"/>
     </row>
@@ -10634,7 +10640,7 @@
         <v>98</v>
       </c>
       <c r="S99" s="3" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="T99" s="8"/>
     </row>
@@ -10696,7 +10702,7 @@
         <v>99</v>
       </c>
       <c r="S100" s="3" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="T100" s="8"/>
     </row>
@@ -10758,7 +10764,7 @@
         <v>100</v>
       </c>
       <c r="S101" s="3" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="T101" s="8"/>
     </row>
@@ -10809,18 +10815,18 @@
         <v>900</v>
       </c>
       <c r="P102" t="str">
-        <f t="shared" ref="P102:P131" si="12">IF(COUNTIF(S102,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" ref="P102:P130" si="12">IF(COUNTIF(S102,"*adj*")&gt;0,"+","-")</f>
         <v>+</v>
       </c>
       <c r="Q102" t="str">
-        <f t="shared" ref="Q102:Q131" si="13">IF(COUNTIF(S102,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" ref="Q102:Q130" si="13">IF(COUNTIF(S102,"*word=*")&gt;0,"-","+")</f>
         <v>+</v>
       </c>
       <c r="R102">
         <v>101</v>
       </c>
       <c r="S102" s="3" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="T102" s="8"/>
     </row>
@@ -10882,7 +10888,7 @@
         <v>102</v>
       </c>
       <c r="S103" s="3" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="T103" s="8"/>
     </row>
@@ -10944,7 +10950,7 @@
         <v>103</v>
       </c>
       <c r="S104" s="3" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="T104" s="8"/>
     </row>
@@ -11006,7 +11012,7 @@
         <v>104</v>
       </c>
       <c r="S105" s="3" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="T105" s="8"/>
     </row>
@@ -11068,7 +11074,7 @@
         <v>105</v>
       </c>
       <c r="S106" s="3" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="T106" s="8"/>
     </row>
@@ -11130,7 +11136,7 @@
         <v>106</v>
       </c>
       <c r="S107" s="3" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="T107" s="8"/>
     </row>
@@ -11192,7 +11198,7 @@
         <v>107</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="T108" s="8"/>
     </row>
@@ -11254,7 +11260,7 @@
         <v>108</v>
       </c>
       <c r="S109" s="3" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="T109" s="8"/>
     </row>
@@ -11316,11 +11322,11 @@
         <v>109</v>
       </c>
       <c r="S110" s="3" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="T110" s="8"/>
       <c r="U110" t="s">
-        <v>1090</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
@@ -11381,7 +11387,7 @@
         <v>110</v>
       </c>
       <c r="S111" s="3" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="T111" s="8"/>
     </row>
@@ -11443,7 +11449,7 @@
         <v>111</v>
       </c>
       <c r="S112" s="3" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="T112" s="8"/>
     </row>
@@ -11505,7 +11511,7 @@
         <v>112</v>
       </c>
       <c r="S113" s="3" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="T113" s="8"/>
     </row>
@@ -11567,7 +11573,7 @@
         <v>113</v>
       </c>
       <c r="S114" s="3" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="T114" s="8"/>
     </row>
@@ -11629,7 +11635,7 @@
         <v>114</v>
       </c>
       <c r="S115" s="3" t="s">
-        <v>1091</v>
+        <v>1089</v>
       </c>
       <c r="T115" s="8"/>
     </row>
@@ -11691,7 +11697,7 @@
         <v>115</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="T116" s="8"/>
     </row>
@@ -11753,7 +11759,7 @@
         <v>116</v>
       </c>
       <c r="S117" s="3" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="T117" s="8"/>
     </row>
@@ -11815,7 +11821,7 @@
         <v>117</v>
       </c>
       <c r="S118" s="3" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="T118" s="8"/>
     </row>
@@ -11877,7 +11883,7 @@
         <v>118</v>
       </c>
       <c r="S119" s="3" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="T119" s="8"/>
     </row>
@@ -11939,11 +11945,11 @@
         <v>119</v>
       </c>
       <c r="S120" s="3" t="s">
-        <v>1092</v>
+        <v>1090</v>
       </c>
       <c r="T120" s="8"/>
       <c r="U120" t="s">
-        <v>1093</v>
+        <v>1091</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
@@ -12004,7 +12010,7 @@
         <v>120</v>
       </c>
       <c r="S121" s="3" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="T121" s="8"/>
     </row>
@@ -12066,7 +12072,7 @@
         <v>121</v>
       </c>
       <c r="S122" s="3" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="T122" s="8"/>
     </row>
@@ -12190,7 +12196,7 @@
         <v>123</v>
       </c>
       <c r="S124" s="3" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="T124" s="8"/>
     </row>
@@ -12252,7 +12258,7 @@
         <v>124</v>
       </c>
       <c r="S125" s="3" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="T125" s="8"/>
     </row>
@@ -12376,7 +12382,7 @@
         <v>126</v>
       </c>
       <c r="S127" s="3" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="T127" s="8"/>
     </row>
@@ -12438,7 +12444,7 @@
         <v>127</v>
       </c>
       <c r="S128" s="3" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="T128" s="8"/>
     </row>
@@ -12500,7 +12506,7 @@
         <v>128</v>
       </c>
       <c r="S129" s="3" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="T129" s="8"/>
     </row>
@@ -12562,98 +12568,100 @@
         <v>129</v>
       </c>
       <c r="S130" s="3" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="T130" s="8"/>
       <c r="U130" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>393</v>
-      </c>
-      <c r="B131">
-        <v>104</v>
-      </c>
-      <c r="C131" t="s">
-        <v>15</v>
-      </c>
-      <c r="D131">
-        <v>239</v>
-      </c>
-      <c r="E131" s="1">
-        <v>5479</v>
-      </c>
-      <c r="F131">
-        <v>2</v>
-      </c>
-      <c r="G131">
-        <v>2</v>
-      </c>
-      <c r="H131">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="132" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A132" s="5"/>
+      <c r="B132" s="5"/>
+      <c r="C132" s="5"/>
+      <c r="D132" s="5"/>
+      <c r="E132" s="5"/>
+      <c r="F132" s="5"/>
+      <c r="G132" s="5"/>
+      <c r="H132" s="5"/>
+      <c r="I132" s="5"/>
+      <c r="J132" s="5"/>
+      <c r="K132" s="5"/>
+      <c r="L132" s="5"/>
+      <c r="M132" s="5"/>
+      <c r="N132" s="5"/>
+      <c r="O132" s="5"/>
+      <c r="P132" s="5"/>
+      <c r="Q132" s="5"/>
+      <c r="R132" s="5"/>
+      <c r="S132" s="5"/>
+      <c r="T132" s="5"/>
+      <c r="U132" s="5"/>
+      <c r="V132" s="5"/>
+    </row>
+    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A134" t="s">
+        <v>651</v>
+      </c>
+      <c r="B134">
+        <v>175</v>
+      </c>
+      <c r="C134" t="s">
+        <v>398</v>
+      </c>
+      <c r="D134">
+        <v>1020</v>
+      </c>
+      <c r="E134" s="1">
+        <v>6928</v>
+      </c>
+      <c r="F134" t="s">
+        <v>179</v>
+      </c>
+      <c r="G134">
+        <v>3</v>
+      </c>
+      <c r="H134">
         <v>16</v>
       </c>
-      <c r="I131">
-        <v>4</v>
-      </c>
-      <c r="J131">
-        <v>12</v>
-      </c>
-      <c r="K131" s="1">
-        <v>2081</v>
-      </c>
-      <c r="L131" t="s">
-        <v>394</v>
-      </c>
-      <c r="M131" t="s">
-        <v>395</v>
-      </c>
-      <c r="N131" t="s">
-        <v>396</v>
-      </c>
-      <c r="O131" s="3" t="s">
-        <v>917</v>
-      </c>
-      <c r="P131" t="str">
-        <f t="shared" si="12"/>
-        <v>+</v>
-      </c>
-      <c r="Q131" t="str">
-        <f t="shared" si="13"/>
-        <v>+</v>
-      </c>
-      <c r="R131">
+      <c r="I134">
+        <v>16</v>
+      </c>
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134" s="1">
+        <v>3147</v>
+      </c>
+      <c r="L134" s="1">
+        <v>1477</v>
+      </c>
+      <c r="M134" t="s">
+        <v>652</v>
+      </c>
+      <c r="N134" t="s">
+        <v>653</v>
+      </c>
+      <c r="O134" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="P134" t="str">
+        <f>IF(COUNTIF(S134,"*adj*")&gt;0,"+","-")</f>
+        <v>+</v>
+      </c>
+      <c r="Q134" t="str">
+        <f>IF(COUNTIF(S134,"*word=*")&gt;0,"-","+")</f>
+        <v>-</v>
+      </c>
+      <c r="R134">
         <v>130</v>
       </c>
-      <c r="S131" s="3" t="s">
-        <v>1049</v>
-      </c>
-      <c r="T131" s="8"/>
-    </row>
-    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A133" s="5"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
-      <c r="E133" s="5"/>
-      <c r="F133" s="5"/>
-      <c r="G133" s="5"/>
-      <c r="H133" s="5"/>
-      <c r="I133" s="5"/>
-      <c r="J133" s="5"/>
-      <c r="K133" s="5"/>
-      <c r="L133" s="5"/>
-      <c r="M133" s="5"/>
-      <c r="N133" s="5"/>
-      <c r="O133" s="5"/>
-      <c r="P133" s="5"/>
-      <c r="Q133" s="5"/>
-      <c r="R133" s="5"/>
-      <c r="S133" s="5"/>
-      <c r="T133" s="5"/>
-      <c r="U133" s="5"/>
-      <c r="V133" s="5"/>
+      <c r="S134" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="T134" s="6" t="s">
+        <v>1181</v>
+      </c>
     </row>
     <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -12713,16 +12721,16 @@
         <v>131</v>
       </c>
       <c r="S135" s="3" t="s">
-        <v>1158</v>
+        <v>1156</v>
       </c>
       <c r="T135" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="U135" s="6" t="s">
-        <v>1066</v>
+        <v>1064</v>
       </c>
       <c r="V135" t="s">
-        <v>1075</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="136" spans="1:22" x14ac:dyDescent="0.25">
@@ -12786,10 +12794,10 @@
         <v>746</v>
       </c>
       <c r="T136" t="s">
-        <v>1100</v>
+        <v>1098</v>
       </c>
       <c r="U136" s="6" t="s">
-        <v>1067</v>
+        <v>1065</v>
       </c>
       <c r="V136" t="s">
         <v>814</v>
@@ -12853,10 +12861,10 @@
         <v>133</v>
       </c>
       <c r="S137" s="3" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="T137" s="6" t="s">
-        <v>1104</v>
+        <v>1102</v>
       </c>
       <c r="V137" t="s">
         <v>919</v>
@@ -12920,13 +12928,13 @@
         <v>134</v>
       </c>
       <c r="S138" s="3" t="s">
-        <v>1058</v>
+        <v>1056</v>
       </c>
       <c r="T138" s="6" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
       <c r="V138" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.25">
@@ -12987,10 +12995,10 @@
         <v>135</v>
       </c>
       <c r="S139" s="3" t="s">
-        <v>1059</v>
+        <v>1057</v>
       </c>
       <c r="T139" s="6" t="s">
-        <v>1105</v>
+        <v>1103</v>
       </c>
       <c r="V139" t="s">
         <v>803</v>
@@ -13054,10 +13062,10 @@
         <v>136</v>
       </c>
       <c r="S140" s="3" t="s">
-        <v>1159</v>
+        <v>1157</v>
       </c>
       <c r="T140" s="6" t="s">
-        <v>1114</v>
+        <v>1112</v>
       </c>
       <c r="V140" t="s">
         <v>922</v>
@@ -13121,10 +13129,10 @@
         <v>137</v>
       </c>
       <c r="S141" s="3" t="s">
-        <v>1161</v>
+        <v>1159</v>
       </c>
       <c r="T141" s="6" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
       <c r="V141" t="s">
         <v>804</v>
@@ -13188,10 +13196,10 @@
         <v>138</v>
       </c>
       <c r="S142" s="3" t="s">
-        <v>1061</v>
+        <v>1059</v>
       </c>
       <c r="T142" s="6" t="s">
-        <v>1106</v>
+        <v>1104</v>
       </c>
       <c r="V142" t="s">
         <v>800</v>
@@ -13255,10 +13263,10 @@
         <v>139</v>
       </c>
       <c r="S143" s="3" t="s">
-        <v>1160</v>
+        <v>1158</v>
       </c>
       <c r="T143" s="6" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
       <c r="V143" t="s">
         <v>924</v>
@@ -13322,10 +13330,10 @@
         <v>140</v>
       </c>
       <c r="S144" s="3" t="s">
-        <v>1162</v>
+        <v>1160</v>
       </c>
       <c r="T144" s="6" t="s">
-        <v>1107</v>
+        <v>1105</v>
       </c>
       <c r="V144" t="s">
         <v>802</v>
@@ -13389,10 +13397,10 @@
         <v>141</v>
       </c>
       <c r="S145" s="3" t="s">
-        <v>1062</v>
+        <v>1060</v>
       </c>
       <c r="T145" s="7" t="s">
-        <v>1108</v>
+        <v>1106</v>
       </c>
       <c r="V145" t="s">
         <v>926</v>
@@ -13456,10 +13464,10 @@
         <v>142</v>
       </c>
       <c r="S146" s="3" t="s">
-        <v>1063</v>
+        <v>1061</v>
       </c>
       <c r="T146" s="7" t="s">
-        <v>1109</v>
+        <v>1107</v>
       </c>
       <c r="V146" t="s">
         <v>928</v>
@@ -13523,10 +13531,10 @@
         <v>143</v>
       </c>
       <c r="S147" s="3" t="s">
-        <v>1064</v>
+        <v>1062</v>
       </c>
       <c r="T147" s="7" t="s">
-        <v>1097</v>
+        <v>1095</v>
       </c>
       <c r="V147" t="s">
         <v>805</v>
@@ -13590,13 +13598,13 @@
         <v>144</v>
       </c>
       <c r="S148" s="3" t="s">
-        <v>1096</v>
+        <v>1094</v>
       </c>
       <c r="T148" s="7" t="s">
-        <v>1102</v>
+        <v>1100</v>
       </c>
       <c r="V148" t="s">
-        <v>1095</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.25">
@@ -13604,21 +13612,21 @@
         <v>648</v>
       </c>
       <c r="P149" t="str">
-        <f>IF(COUNTIF(S149,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" ref="P149:P154" si="16">IF(COUNTIF(S149,"*adj*")&gt;0,"+","-")</f>
         <v>+</v>
       </c>
       <c r="Q149" t="str">
-        <f>IF(COUNTIF(S149,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" ref="Q149:Q154" si="17">IF(COUNTIF(S149,"*word=*")&gt;0,"-","+")</f>
         <v>+</v>
       </c>
       <c r="R149">
         <v>145</v>
       </c>
       <c r="S149" s="3" t="s">
-        <v>1119</v>
+        <v>1117</v>
       </c>
       <c r="T149" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="V149" t="s">
         <v>820</v>
@@ -13671,21 +13679,21 @@
         <v>798</v>
       </c>
       <c r="P150" t="str">
-        <f>IF(COUNTIF(S150,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="16"/>
         <v>+</v>
       </c>
       <c r="Q150" t="str">
-        <f>IF(COUNTIF(S150,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="17"/>
         <v>+</v>
       </c>
       <c r="R150">
         <v>146</v>
       </c>
       <c r="S150" s="3" t="s">
-        <v>1120</v>
+        <v>1118</v>
       </c>
       <c r="T150" t="s">
-        <v>1110</v>
+        <v>1108</v>
       </c>
       <c r="V150" t="s">
         <v>821</v>
@@ -13738,21 +13746,21 @@
         <v>929</v>
       </c>
       <c r="P151" t="str">
-        <f>IF(COUNTIF(S151,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="16"/>
         <v>+</v>
       </c>
       <c r="Q151" t="str">
-        <f>IF(COUNTIF(S151,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="17"/>
         <v>+</v>
       </c>
       <c r="R151">
         <v>147</v>
       </c>
       <c r="S151" s="3" t="s">
-        <v>1163</v>
+        <v>1161</v>
       </c>
       <c r="T151" t="s">
-        <v>1098</v>
+        <v>1096</v>
       </c>
       <c r="V151" t="s">
         <v>930</v>
@@ -13805,21 +13813,21 @@
         <v>931</v>
       </c>
       <c r="P152" t="str">
-        <f>IF(COUNTIF(S152,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="16"/>
         <v>+</v>
       </c>
       <c r="Q152" t="str">
-        <f>IF(COUNTIF(S152,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="17"/>
         <v>+</v>
       </c>
       <c r="R152">
         <v>148</v>
       </c>
       <c r="S152" s="3" t="s">
-        <v>1126</v>
+        <v>1124</v>
       </c>
       <c r="T152" t="s">
-        <v>1111</v>
+        <v>1109</v>
       </c>
       <c r="V152" t="s">
         <v>932</v>
@@ -13872,21 +13880,21 @@
         <v>933</v>
       </c>
       <c r="P153" t="str">
-        <f>IF(COUNTIF(S153,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="16"/>
         <v>+</v>
       </c>
       <c r="Q153" t="str">
-        <f>IF(COUNTIF(S153,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="17"/>
         <v>+</v>
       </c>
       <c r="R153">
         <v>149</v>
       </c>
       <c r="S153" s="3" t="s">
-        <v>1164</v>
+        <v>1162</v>
       </c>
       <c r="T153" t="s">
-        <v>1099</v>
+        <v>1097</v>
       </c>
       <c r="V153" t="s">
         <v>934</v>
@@ -13939,21 +13947,21 @@
         <v>935</v>
       </c>
       <c r="P154" t="str">
-        <f>IF(COUNTIF(S154,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="16"/>
         <v>+</v>
       </c>
       <c r="Q154" t="str">
-        <f>IF(COUNTIF(S154,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="17"/>
         <v>+</v>
       </c>
       <c r="R154">
         <v>150</v>
       </c>
       <c r="S154" s="3" t="s">
-        <v>1128</v>
+        <v>1126</v>
       </c>
       <c r="T154" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="V154" t="s">
         <v>936</v>
@@ -14017,10 +14025,10 @@
         <v>151</v>
       </c>
       <c r="S155" s="3" t="s">
-        <v>1129</v>
+        <v>1127</v>
       </c>
       <c r="T155" t="s">
-        <v>1130</v>
+        <v>1128</v>
       </c>
       <c r="V155" t="s">
         <v>823</v>
@@ -14084,10 +14092,10 @@
         <v>152</v>
       </c>
       <c r="S156" s="3" t="s">
-        <v>1131</v>
+        <v>1129</v>
       </c>
       <c r="T156" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
       <c r="V156" t="s">
         <v>824</v>
@@ -14151,10 +14159,10 @@
         <v>153</v>
       </c>
       <c r="S157" s="3" t="s">
-        <v>1132</v>
+        <v>1130</v>
       </c>
       <c r="T157" t="s">
-        <v>1112</v>
+        <v>1110</v>
       </c>
       <c r="V157" t="s">
         <v>938</v>
@@ -14218,10 +14226,10 @@
         <v>154</v>
       </c>
       <c r="S158" s="3" t="s">
-        <v>1165</v>
+        <v>1163</v>
       </c>
       <c r="T158" t="s">
-        <v>1133</v>
+        <v>1131</v>
       </c>
       <c r="V158" t="s">
         <v>825</v>
@@ -14285,10 +14293,10 @@
         <v>155</v>
       </c>
       <c r="S159" s="3" t="s">
-        <v>1134</v>
+        <v>1132</v>
       </c>
       <c r="T159" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="V159" t="s">
         <v>940</v>
@@ -14352,10 +14360,10 @@
         <v>156</v>
       </c>
       <c r="S160" s="3" t="s">
-        <v>1135</v>
+        <v>1133</v>
       </c>
       <c r="T160" t="s">
-        <v>1113</v>
+        <v>1111</v>
       </c>
       <c r="V160" t="s">
         <v>810</v>
@@ -14419,10 +14427,10 @@
         <v>157</v>
       </c>
       <c r="S161" s="3" t="s">
-        <v>1137</v>
+        <v>1135</v>
       </c>
       <c r="T161" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="V161" t="s">
         <v>806</v>
@@ -14486,10 +14494,10 @@
         <v>158</v>
       </c>
       <c r="S162" s="3" t="s">
-        <v>1138</v>
+        <v>1136</v>
       </c>
       <c r="T162" t="s">
-        <v>1121</v>
+        <v>1119</v>
       </c>
       <c r="V162" t="s">
         <v>801</v>
@@ -14553,10 +14561,10 @@
         <v>159</v>
       </c>
       <c r="S163" s="3" t="s">
-        <v>1139</v>
+        <v>1137</v>
       </c>
       <c r="T163" t="s">
-        <v>1122</v>
+        <v>1120</v>
       </c>
       <c r="V163" t="s">
         <v>807</v>
@@ -14620,10 +14628,10 @@
         <v>160</v>
       </c>
       <c r="S164" s="3" t="s">
-        <v>1140</v>
+        <v>1138</v>
       </c>
       <c r="T164" t="s">
-        <v>1123</v>
+        <v>1121</v>
       </c>
       <c r="V164" t="s">
         <v>828</v>
@@ -14687,10 +14695,10 @@
         <v>161</v>
       </c>
       <c r="S165" s="3" t="s">
-        <v>1166</v>
+        <v>1164</v>
       </c>
       <c r="T165" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
       <c r="V165" t="s">
         <v>811</v>
@@ -14754,10 +14762,10 @@
         <v>162</v>
       </c>
       <c r="S166" s="3" t="s">
-        <v>1141</v>
+        <v>1139</v>
       </c>
       <c r="T166" t="s">
-        <v>1142</v>
+        <v>1140</v>
       </c>
       <c r="V166" t="s">
         <v>812</v>
@@ -14821,10 +14829,10 @@
         <v>163</v>
       </c>
       <c r="S167" s="3" t="s">
-        <v>1143</v>
+        <v>1141</v>
       </c>
       <c r="T167" t="s">
-        <v>1125</v>
+        <v>1123</v>
       </c>
       <c r="V167" t="s">
         <v>813</v>
@@ -14888,10 +14896,10 @@
         <v>164</v>
       </c>
       <c r="S168" s="3" t="s">
-        <v>1144</v>
+        <v>1142</v>
       </c>
       <c r="T168" t="s">
-        <v>1145</v>
+        <v>1143</v>
       </c>
       <c r="V168" t="s">
         <v>942</v>
@@ -14955,10 +14963,10 @@
         <v>165</v>
       </c>
       <c r="S169" s="3" t="s">
-        <v>1146</v>
+        <v>1144</v>
       </c>
       <c r="T169" t="s">
-        <v>1103</v>
+        <v>1101</v>
       </c>
       <c r="V169" t="s">
         <v>809</v>
@@ -15022,10 +15030,10 @@
         <v>166</v>
       </c>
       <c r="S170" s="3" t="s">
-        <v>1148</v>
+        <v>1146</v>
       </c>
       <c r="T170" t="s">
-        <v>1149</v>
+        <v>1147</v>
       </c>
       <c r="V170" t="s">
         <v>818</v>
@@ -15089,10 +15097,10 @@
         <v>167</v>
       </c>
       <c r="S171" s="3" t="s">
-        <v>1167</v>
+        <v>1165</v>
       </c>
       <c r="T171" t="s">
-        <v>1150</v>
+        <v>1148</v>
       </c>
       <c r="V171" t="s">
         <v>799</v>
@@ -15156,10 +15164,10 @@
         <v>168</v>
       </c>
       <c r="S172" s="3" t="s">
-        <v>1151</v>
+        <v>1149</v>
       </c>
       <c r="T172" t="s">
-        <v>1152</v>
+        <v>1150</v>
       </c>
       <c r="V172" t="s">
         <v>817</v>
@@ -15223,10 +15231,10 @@
         <v>169</v>
       </c>
       <c r="S173" s="3" t="s">
-        <v>1153</v>
+        <v>1151</v>
       </c>
       <c r="T173" t="s">
-        <v>1124</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.25">
@@ -15287,10 +15295,10 @@
         <v>170</v>
       </c>
       <c r="S174" s="3" t="s">
-        <v>1154</v>
+        <v>1152</v>
       </c>
       <c r="T174" t="s">
-        <v>1155</v>
+        <v>1153</v>
       </c>
       <c r="V174" t="s">
         <v>819</v>
@@ -15343,11 +15351,11 @@
         <v>833</v>
       </c>
       <c r="P175" t="str">
-        <f>IF(COUNTIF(S175,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" ref="P175:P187" si="18">IF(COUNTIF(S175,"*adj*")&gt;0,"+","-")</f>
         <v>-</v>
       </c>
       <c r="Q175" t="str">
-        <f>IF(COUNTIF(S175,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" ref="Q175:Q187" si="19">IF(COUNTIF(S175,"*word=*")&gt;0,"-","+")</f>
         <v>+</v>
       </c>
       <c r="R175">
@@ -15357,7 +15365,7 @@
         <v>833</v>
       </c>
       <c r="T175" t="s">
-        <v>1115</v>
+        <v>1113</v>
       </c>
       <c r="V175" t="s">
         <v>944</v>
@@ -15410,21 +15418,21 @@
         <v>836</v>
       </c>
       <c r="P176" t="str">
-        <f>IF(COUNTIF(S176,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q176" t="str">
-        <f>IF(COUNTIF(S176,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R176">
         <v>172</v>
       </c>
       <c r="S176" s="3" t="s">
-        <v>1147</v>
+        <v>1145</v>
       </c>
       <c r="T176" t="s">
-        <v>1101</v>
+        <v>1099</v>
       </c>
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.25">
@@ -15474,21 +15482,21 @@
         <v>858</v>
       </c>
       <c r="P177" t="str">
-        <f>IF(COUNTIF(S177,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q177" t="str">
-        <f>IF(COUNTIF(S177,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R177">
         <v>173</v>
       </c>
       <c r="S177" s="3" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="T177" s="6" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.25">
@@ -15538,21 +15546,21 @@
         <v>864</v>
       </c>
       <c r="P178" t="str">
-        <f>IF(COUNTIF(S178,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q178" t="str">
-        <f>IF(COUNTIF(S178,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R178">
         <v>174</v>
       </c>
       <c r="S178" s="3" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="T178" s="6" t="s">
-        <v>1074</v>
+        <v>1072</v>
       </c>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.25">
@@ -15602,21 +15610,21 @@
         <v>865</v>
       </c>
       <c r="P179" t="str">
-        <f>IF(COUNTIF(S179,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q179" t="str">
-        <f>IF(COUNTIF(S179,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R179">
         <v>175</v>
       </c>
       <c r="S179" s="3" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="T179" s="6" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.25">
@@ -15666,21 +15674,21 @@
         <v>866</v>
       </c>
       <c r="P180" t="str">
-        <f>IF(COUNTIF(S180,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q180" t="str">
-        <f>IF(COUNTIF(S180,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R180">
         <v>176</v>
       </c>
       <c r="S180" s="3" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="T180" s="6" t="s">
-        <v>1168</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.25">
@@ -15730,65 +15738,65 @@
         <v>740</v>
       </c>
       <c r="P181" t="str">
-        <f>IF(COUNTIF(S181,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q181" t="str">
-        <f>IF(COUNTIF(S181,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R181">
         <v>177</v>
       </c>
       <c r="S181" s="3" t="s">
-        <v>1169</v>
+        <v>1167</v>
       </c>
       <c r="T181" s="6" t="s">
-        <v>1086</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>1117</v>
+        <v>1115</v>
       </c>
       <c r="P182" t="str">
-        <f>IF(COUNTIF(S182,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q182" t="str">
-        <f>IF(COUNTIF(S182,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R182">
         <v>178</v>
       </c>
       <c r="S182" s="3" t="s">
-        <v>1081</v>
+        <v>1079</v>
       </c>
       <c r="T182" t="s">
-        <v>1082</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>1118</v>
+        <v>1116</v>
       </c>
       <c r="P183" t="str">
-        <f>IF(COUNTIF(S183,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q183" t="str">
-        <f>IF(COUNTIF(S183,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R183">
         <v>179</v>
       </c>
       <c r="S183" s="3" t="s">
-        <v>1170</v>
+        <v>1168</v>
       </c>
       <c r="T183" t="s">
-        <v>1085</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.25">
@@ -15796,21 +15804,21 @@
         <v>337</v>
       </c>
       <c r="P184" t="str">
-        <f>IF(COUNTIF(S184,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q184" t="str">
-        <f>IF(COUNTIF(S184,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R184">
         <v>180</v>
       </c>
       <c r="S184" s="3" t="s">
-        <v>1087</v>
+        <v>1085</v>
       </c>
       <c r="T184" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.25">
@@ -15860,21 +15868,21 @@
         <v>898</v>
       </c>
       <c r="P185" t="str">
-        <f>IF(COUNTIF(S185,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q185" t="str">
-        <f>IF(COUNTIF(S185,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R185">
         <v>181</v>
       </c>
       <c r="S185" s="3" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="T185" t="s">
-        <v>1088</v>
+        <v>1086</v>
       </c>
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.25">
@@ -15924,21 +15932,21 @@
         <v>899</v>
       </c>
       <c r="P186" t="str">
-        <f>IF(COUNTIF(S186,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>+</v>
       </c>
       <c r="Q186" t="str">
-        <f>IF(COUNTIF(S186,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R186">
         <v>182</v>
       </c>
       <c r="S186" s="3" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="T186" t="s">
-        <v>1089</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.25">
@@ -15988,21 +15996,21 @@
         <v>774</v>
       </c>
       <c r="P187" t="str">
-        <f>IF(COUNTIF(S187,"*adj*")&gt;0,"+","-")</f>
+        <f t="shared" si="18"/>
         <v>-</v>
       </c>
       <c r="Q187" t="str">
-        <f>IF(COUNTIF(S187,"*word=*")&gt;0,"-","+")</f>
+        <f t="shared" si="19"/>
         <v>+</v>
       </c>
       <c r="R187">
         <v>183</v>
       </c>
       <c r="S187" s="3" t="s">
-        <v>1176</v>
+        <v>1174</v>
       </c>
       <c r="T187" t="s">
-        <v>1172</v>
+        <v>1170</v>
       </c>
     </row>
     <row r="188" spans="1:22" x14ac:dyDescent="0.25">
@@ -16089,13 +16097,13 @@
         <v>184</v>
       </c>
       <c r="S191" s="3" t="s">
-        <v>1136</v>
+        <v>1134</v>
       </c>
       <c r="T191" t="s">
-        <v>1177</v>
+        <v>1175</v>
       </c>
       <c r="U191" t="s">
-        <v>1180</v>
+        <v>1178</v>
       </c>
     </row>
     <row r="192" spans="1:22" x14ac:dyDescent="0.25">
@@ -16156,10 +16164,10 @@
         <v>185</v>
       </c>
       <c r="S192" s="3" t="s">
-        <v>1171</v>
+        <v>1169</v>
       </c>
       <c r="T192" t="s">
-        <v>1175</v>
+        <v>1173</v>
       </c>
       <c r="V192" t="s">
         <v>827</v>
@@ -16223,10 +16231,10 @@
         <v>186</v>
       </c>
       <c r="S193" s="3" t="s">
-        <v>1173</v>
+        <v>1171</v>
       </c>
       <c r="T193" t="s">
-        <v>1174</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
@@ -16310,13 +16318,13 @@
         <v>187</v>
       </c>
       <c r="S197" s="3" t="s">
-        <v>1127</v>
+        <v>1125</v>
       </c>
       <c r="T197" t="s">
-        <v>1178</v>
+        <v>1176</v>
       </c>
       <c r="U197" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
@@ -16335,13 +16343,13 @@
         <v>188</v>
       </c>
       <c r="S198" s="9" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="T198" t="s">
-        <v>1116</v>
+        <v>1114</v>
       </c>
       <c r="U198" t="s">
-        <v>1179</v>
+        <v>1177</v>
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
@@ -16564,7 +16572,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>T1 R1 P1:Q131 P191:Q193 P200:P1048576 P197:Q198 P135:Q187</xm:sqref>
+          <xm:sqref>T1 R1 P191:Q193 P200:P1048576 P197:Q198 P134:Q187 P1:Q130</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
finished adding idioms - crosstable completed
</commit_message>
<xml_diff>
--- a/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
+++ b/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\idiom_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07481172-A30E-403D-B5AD-568C5A1FBE83}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4B053B-1B9F-4C19-8174-9FD0949C81A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="idiom_database" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">idiom_database!$A$1:$S$237</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">idiom_database!$A$1:$S$233</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1479" uniqueCount="1182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1474" uniqueCount="1176">
   <si>
     <t>Idiom</t>
   </si>
@@ -2514,9 +2514,6 @@
     <t>([ word = "aan" ] [ pos_head = "lid" ] [ word = "aarde" ] [ lemma = "toevertrouwen" ])|([ lemma = "vertrouwen" ] [ word = "aan" ] [ pos_head = "lid" ] [ word = "aarde" ] [word = "toe"])</t>
   </si>
   <si>
-    <t>(([ word = "aan" ] [ pos_head = "lid" ] [ pos_head = "adj" ]? [ word = "aarde" ] [ lemma = "toevertrouwen" ])|([ lemma = "vertrouwen" ] [ word = "aan" ] [ pos_head = "lid" ] [ pos_head = "adj" ]? [ word = "aarde" ] [word = "toe"]))|</t>
-  </si>
-  <si>
     <t>(([lemma="wippen"] []{1,3} [lemma="uit"][pos_head="lid"] [lemma="zadel"])|([lemma="uit"][pos_head="lid"][lemma="zadel"][lemma="wippen"]))|</t>
   </si>
   <si>
@@ -3225,12 +3222,6 @@
     <t>verb regex</t>
   </si>
   <si>
-    <t>\\bhouden\\s|\\bgehouden\\s|\\bhoudt\\s|\\bhielden\\s</t>
-  </si>
-  <si>
-    <t>\\bhalen\\s|\\bhalen\\s|\\bhalen\\s|\\bhalen\\s|\\bhalen\\s</t>
-  </si>
-  <si>
     <t>[ lemma= "kat" ] [ lemma= "op" ] [ pos_head = "lid" ] [ pos_head = "adj" ]? [ lemma= "spek" ]</t>
   </si>
   <si>
@@ -3279,9 +3270,6 @@
     <t>[ lemma= "pas"] [ lemma= "op" ] [ lemma = "de" ] [ lemma= "plaats" ]</t>
   </si>
   <si>
-    <t>[pos_head = "vnw"] [lemma= "uit" ] [ pos_head="lid" ] [pos_head = "adj"]? [ word= "voeten" ]</t>
-  </si>
-  <si>
     <t>slaan</t>
   </si>
   <si>
@@ -3531,45 +3519,24 @@
     <t>[ lemma= "op" ] [ pos_head="vnw" | pos_head="lid" ] [ pos_head = "adj" ]? [ lemma= "ziel" ]</t>
   </si>
   <si>
-    <t>houden  (/ hebben?)</t>
-  </si>
-  <si>
     <t>[ lemma= "in" ] [ pos_head= "vnw" | pos_head = "lid" ] [ pos_head = "adj" ]? [ lemma= "keel" ]</t>
   </si>
   <si>
     <t>[ lemma= "om" ] [pos_head = "vnw"|"lid"] [ pos_head = "adj" ]? [ lemma= "hart" ]</t>
   </si>
   <si>
-    <t>[  word = "door"  ] [  pos_head = "lid"  ] [ pos_head = "adj" ]? [  lemma = "kerk"  ]</t>
-  </si>
-  <si>
     <t>gaan</t>
   </si>
   <si>
     <t>[ lemma= "in" ] [pos_head = "vnw"|"lid"] [ pos_head = "adj" ]? [ lemma= "mond" ]</t>
   </si>
   <si>
-    <t>lopen, water</t>
-  </si>
-  <si>
-    <t>kogel, zijn</t>
-  </si>
-  <si>
     <t>[lemma != "kort"][ lemma= "door" ] [ pos_head="lid" ] [ lemma= "bocht" ]</t>
   </si>
   <si>
-    <t xml:space="preserve">toevertrouwen </t>
-  </si>
-  <si>
     <t>snijden</t>
   </si>
   <si>
-    <t>kan letterljijk zijn</t>
-  </si>
-  <si>
-    <t>zoek op vertrouwen zonder letterlijke woordgrenzen</t>
-  </si>
-  <si>
     <t>[ word = "gaatje" ] [ lemma= "in" ] [pos_head = "lid" | pos_head = "vnw"] [ pos_head = "adj" ]? [ lemma= "hoofd" ]</t>
   </si>
   <si>
@@ -3577,6 +3544,21 @@
   </si>
   <si>
     <t>maken</t>
+  </si>
+  <si>
+    <t>toevertrouwen / vertrouwen</t>
+  </si>
+  <si>
+    <t>houden  / hebben</t>
+  </si>
+  <si>
+    <t>[lemma="kogel"][]{0,3}[lemma="door"][pos_head="lid"][lemma="kerk"]</t>
+  </si>
+  <si>
+    <t>[lemma= "uit" ] [ pos_head="lid" ] [pos_head = "adj"]? [ word= "voeten" ]</t>
+  </si>
+  <si>
+    <t>kan letterljijk zijn - weggelaten - nog rapporteren</t>
   </si>
 </sst>
 </file>
@@ -4087,7 +4069,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -4100,6 +4082,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4145,7 +4128,21 @@
     <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -4473,10 +4470,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V237"/>
+  <dimension ref="A1:V233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="S147" sqref="S147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4494,8 +4491,8 @@
     <col min="13" max="13" width="54.28515625" hidden="1" customWidth="1"/>
     <col min="14" max="14" width="112.5703125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="202.85546875" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5703125" customWidth="1"/>
-    <col min="17" max="17" width="28" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="28" hidden="1" customWidth="1"/>
     <col min="18" max="18" width="19.5703125" customWidth="1"/>
     <col min="19" max="19" width="129" customWidth="1"/>
     <col min="20" max="20" width="68.28515625" customWidth="1"/>
@@ -4550,22 +4547,22 @@
         <v>723</v>
       </c>
       <c r="P1" t="s">
-        <v>1155</v>
+        <v>1151</v>
       </c>
       <c r="Q1" t="s">
-        <v>1154</v>
+        <v>1150</v>
       </c>
       <c r="R1" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="S1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="T1" s="6" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="V1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
@@ -4612,7 +4609,7 @@
         <v>257</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="P2" t="str">
         <f t="shared" ref="P2:P6" si="0">IF(COUNTIF(S2,"*adj*")&gt;0,"+","-")</f>
@@ -4626,7 +4623,7 @@
         <v>1</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>1068</v>
+        <v>1065</v>
       </c>
       <c r="T2" s="8"/>
     </row>
@@ -4674,7 +4671,7 @@
         <v>150</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="P3" t="str">
         <f t="shared" si="0"/>
@@ -4688,7 +4685,7 @@
         <v>2</v>
       </c>
       <c r="S3" s="3" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="T3" s="8"/>
     </row>
@@ -4736,7 +4733,7 @@
         <v>113</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="P4" t="str">
         <f t="shared" si="0"/>
@@ -4750,7 +4747,7 @@
         <v>3</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="T4" s="8"/>
     </row>
@@ -4798,7 +4795,7 @@
         <v>267</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="P5" t="str">
         <f t="shared" si="0"/>
@@ -4812,7 +4809,7 @@
         <v>4</v>
       </c>
       <c r="S5" s="3" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="T5" s="8"/>
     </row>
@@ -4874,7 +4871,7 @@
         <v>5</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>1066</v>
+        <v>1063</v>
       </c>
       <c r="T6" s="8"/>
     </row>
@@ -4936,7 +4933,7 @@
         <v>6</v>
       </c>
       <c r="S7" s="3" t="s">
-        <v>1067</v>
+        <v>1064</v>
       </c>
       <c r="T7" s="8"/>
     </row>
@@ -5045,7 +5042,7 @@
         <v>560</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="P9" t="str">
         <f t="shared" si="2"/>
@@ -5059,7 +5056,7 @@
         <v>8</v>
       </c>
       <c r="S9" s="3" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
@@ -5106,7 +5103,7 @@
         <v>313</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="P10" t="str">
         <f t="shared" si="2"/>
@@ -5120,7 +5117,7 @@
         <v>9</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="11" spans="1:22" x14ac:dyDescent="0.25">
@@ -5229,7 +5226,7 @@
         <v>212</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="P12" t="str">
         <f t="shared" si="2"/>
@@ -5243,7 +5240,7 @@
         <v>11</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="T12" s="8"/>
     </row>
@@ -5291,7 +5288,7 @@
         <v>307</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="P13" t="str">
         <f t="shared" si="2"/>
@@ -5305,7 +5302,7 @@
         <v>12</v>
       </c>
       <c r="S13" s="3" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="T13" s="8"/>
     </row>
@@ -5353,7 +5350,7 @@
         <v>492</v>
       </c>
       <c r="O14" s="3" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="P14" t="str">
         <f t="shared" si="2"/>
@@ -5367,7 +5364,7 @@
         <v>13</v>
       </c>
       <c r="S14" s="3" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="T14" s="8"/>
     </row>
@@ -5415,7 +5412,7 @@
         <v>77</v>
       </c>
       <c r="O15" s="3" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="P15" t="str">
         <f t="shared" si="2"/>
@@ -5429,7 +5426,7 @@
         <v>14</v>
       </c>
       <c r="S15" s="3" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="T15" s="8"/>
     </row>
@@ -5477,7 +5474,7 @@
         <v>400</v>
       </c>
       <c r="O16" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="P16" t="str">
         <f t="shared" si="2"/>
@@ -5491,7 +5488,7 @@
         <v>15</v>
       </c>
       <c r="S16" s="3" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="T16" s="8"/>
     </row>
@@ -5539,7 +5536,7 @@
         <v>424</v>
       </c>
       <c r="O17" s="3" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="P17" t="str">
         <f t="shared" si="2"/>
@@ -5553,7 +5550,7 @@
         <v>16</v>
       </c>
       <c r="S17" s="3" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="T17" s="8"/>
     </row>
@@ -5601,7 +5598,7 @@
         <v>126</v>
       </c>
       <c r="O18" s="3" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="P18" t="str">
         <f t="shared" si="2"/>
@@ -5615,7 +5612,7 @@
         <v>17</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="T18" s="8"/>
     </row>
@@ -5663,7 +5660,7 @@
         <v>549</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="P19" t="str">
         <f t="shared" si="2"/>
@@ -5677,7 +5674,7 @@
         <v>18</v>
       </c>
       <c r="S19" s="3" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="T19" s="8"/>
     </row>
@@ -5725,7 +5722,7 @@
         <v>146</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="P20" t="str">
         <f t="shared" si="2"/>
@@ -5739,7 +5736,7 @@
         <v>19</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="T20" s="8"/>
     </row>
@@ -5787,7 +5784,7 @@
         <v>243</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="P21" t="str">
         <f t="shared" si="2"/>
@@ -5801,7 +5798,7 @@
         <v>20</v>
       </c>
       <c r="S21" s="3" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="T21" s="8"/>
     </row>
@@ -5863,7 +5860,7 @@
         <v>21</v>
       </c>
       <c r="S22" s="3" t="s">
-        <v>1070</v>
+        <v>1067</v>
       </c>
       <c r="T22" s="8"/>
     </row>
@@ -5911,7 +5908,7 @@
         <v>383</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="P23" t="str">
         <f t="shared" si="2"/>
@@ -5925,7 +5922,7 @@
         <v>22</v>
       </c>
       <c r="S23" s="3" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="T23" s="8"/>
     </row>
@@ -5987,7 +5984,7 @@
         <v>23</v>
       </c>
       <c r="S24" s="3" t="s">
-        <v>1069</v>
+        <v>1066</v>
       </c>
       <c r="T24" s="8"/>
     </row>
@@ -6035,7 +6032,7 @@
         <v>515</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="P25" t="str">
         <f t="shared" si="2"/>
@@ -6049,7 +6046,7 @@
         <v>24</v>
       </c>
       <c r="S25" s="3" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="T25" s="8"/>
     </row>
@@ -6097,7 +6094,7 @@
         <v>371</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="P26" t="str">
         <f t="shared" si="2"/>
@@ -6111,7 +6108,7 @@
         <v>25</v>
       </c>
       <c r="S26" s="3" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="T26" s="8"/>
     </row>
@@ -6159,7 +6156,7 @@
         <v>367</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="P27" t="str">
         <f t="shared" si="2"/>
@@ -6173,7 +6170,7 @@
         <v>26</v>
       </c>
       <c r="S27" s="3" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="T27" s="8"/>
     </row>
@@ -6235,7 +6232,7 @@
         <v>27</v>
       </c>
       <c r="S28" s="3" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="T28" s="8"/>
     </row>
@@ -6297,7 +6294,7 @@
         <v>28</v>
       </c>
       <c r="S29" s="3" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="T29" s="8"/>
     </row>
@@ -6345,7 +6342,7 @@
         <v>264</v>
       </c>
       <c r="O30" s="3" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="P30" t="str">
         <f t="shared" si="2"/>
@@ -6359,7 +6356,7 @@
         <v>29</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="T30" s="8"/>
     </row>
@@ -6421,7 +6418,7 @@
         <v>30</v>
       </c>
       <c r="S31" s="3" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="T31" s="8"/>
     </row>
@@ -6483,11 +6480,11 @@
         <v>31</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>1179</v>
+        <v>1168</v>
       </c>
       <c r="T32" s="8"/>
       <c r="U32" t="s">
-        <v>1092</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.25">
@@ -6548,7 +6545,7 @@
         <v>32</v>
       </c>
       <c r="S33" s="3" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="T33" s="8"/>
     </row>
@@ -6596,7 +6593,7 @@
         <v>165</v>
       </c>
       <c r="O34" s="3" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="P34" t="str">
         <f t="shared" si="2"/>
@@ -6610,7 +6607,7 @@
         <v>33</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="T34" s="8"/>
     </row>
@@ -6658,7 +6655,7 @@
         <v>595</v>
       </c>
       <c r="O35" s="3" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="P35" t="str">
         <f t="shared" si="2"/>
@@ -6672,7 +6669,7 @@
         <v>34</v>
       </c>
       <c r="S35" s="3" t="s">
-        <v>1180</v>
+        <v>1169</v>
       </c>
       <c r="T35" s="8"/>
     </row>
@@ -6720,7 +6717,7 @@
         <v>184</v>
       </c>
       <c r="O36" s="3" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="P36" t="str">
         <f t="shared" si="2"/>
@@ -6734,7 +6731,7 @@
         <v>35</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="T36" s="8"/>
     </row>
@@ -6782,7 +6779,7 @@
         <v>354</v>
       </c>
       <c r="O37" s="3" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="P37" t="str">
         <f t="shared" si="2"/>
@@ -6796,7 +6793,7 @@
         <v>36</v>
       </c>
       <c r="S37" s="3" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="T37" s="8"/>
     </row>
@@ -6906,7 +6903,7 @@
         <v>378</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="P39" t="str">
         <f t="shared" ref="P39:P69" si="4">IF(COUNTIF(S39,"*adj*")&gt;0,"+","-")</f>
@@ -6920,7 +6917,7 @@
         <v>38</v>
       </c>
       <c r="S39" s="3" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="T39" s="8"/>
     </row>
@@ -6982,7 +6979,7 @@
         <v>39</v>
       </c>
       <c r="S40" s="3" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="T40" s="8"/>
     </row>
@@ -7030,7 +7027,7 @@
         <v>642</v>
       </c>
       <c r="O41" s="3" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="P41" t="str">
         <f t="shared" si="4"/>
@@ -7044,7 +7041,7 @@
         <v>40</v>
       </c>
       <c r="S41" s="3" t="s">
-        <v>1071</v>
+        <v>1068</v>
       </c>
       <c r="T41" s="8"/>
     </row>
@@ -7092,7 +7089,7 @@
         <v>291</v>
       </c>
       <c r="O42" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="P42" t="str">
         <f t="shared" si="4"/>
@@ -7106,7 +7103,7 @@
         <v>41</v>
       </c>
       <c r="S42" s="3" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="T42" s="8"/>
     </row>
@@ -7154,7 +7151,7 @@
         <v>174</v>
       </c>
       <c r="O43" s="3" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="P43" t="str">
         <f t="shared" si="4"/>
@@ -7168,7 +7165,7 @@
         <v>42</v>
       </c>
       <c r="S43" s="3" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="T43" s="8"/>
     </row>
@@ -7216,7 +7213,7 @@
         <v>332</v>
       </c>
       <c r="O44" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="P44" t="str">
         <f t="shared" si="4"/>
@@ -7230,7 +7227,7 @@
         <v>43</v>
       </c>
       <c r="S44" s="3" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="T44" s="8"/>
     </row>
@@ -7292,7 +7289,7 @@
         <v>44</v>
       </c>
       <c r="S45" s="3" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="T45" s="8"/>
     </row>
@@ -7340,7 +7337,7 @@
         <v>271</v>
       </c>
       <c r="O46" s="3" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="P46" t="str">
         <f t="shared" si="4"/>
@@ -7354,7 +7351,7 @@
         <v>45</v>
       </c>
       <c r="S46" s="3" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="T46" s="8"/>
     </row>
@@ -7526,7 +7523,7 @@
         <v>598</v>
       </c>
       <c r="O49" s="3" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="P49" t="str">
         <f t="shared" si="4"/>
@@ -7540,7 +7537,7 @@
         <v>48</v>
       </c>
       <c r="S49" s="3" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="T49" s="8"/>
     </row>
@@ -7588,7 +7585,7 @@
         <v>58</v>
       </c>
       <c r="O50" s="3" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="P50" t="str">
         <f t="shared" si="4"/>
@@ -7602,7 +7599,7 @@
         <v>49</v>
       </c>
       <c r="S50" s="3" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="T50" s="8"/>
     </row>
@@ -7664,7 +7661,7 @@
         <v>50</v>
       </c>
       <c r="S51" s="3" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="T51" s="8"/>
     </row>
@@ -7726,7 +7723,7 @@
         <v>51</v>
       </c>
       <c r="S52" s="3" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="T52" s="8"/>
     </row>
@@ -7774,7 +7771,7 @@
         <v>81</v>
       </c>
       <c r="O53" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="P53" t="str">
         <f t="shared" si="4"/>
@@ -7788,7 +7785,7 @@
         <v>52</v>
       </c>
       <c r="S53" s="3" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="T53" s="8"/>
     </row>
@@ -7850,7 +7847,7 @@
         <v>53</v>
       </c>
       <c r="S54" s="3" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="T54" s="8"/>
     </row>
@@ -7912,7 +7909,7 @@
         <v>54</v>
       </c>
       <c r="S55" s="3" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="T55" s="8"/>
     </row>
@@ -7974,7 +7971,7 @@
         <v>55</v>
       </c>
       <c r="S56" s="3" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="T56" s="8"/>
     </row>
@@ -8022,7 +8019,7 @@
         <v>656</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="P57" t="str">
         <f t="shared" si="4"/>
@@ -8036,7 +8033,7 @@
         <v>56</v>
       </c>
       <c r="S57" s="3" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="T57" s="8"/>
     </row>
@@ -8098,7 +8095,7 @@
         <v>57</v>
       </c>
       <c r="S58" s="3" t="s">
-        <v>1074</v>
+        <v>1071</v>
       </c>
       <c r="T58" s="8"/>
     </row>
@@ -8146,7 +8143,7 @@
         <v>171</v>
       </c>
       <c r="O59" s="3" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="P59" t="str">
         <f t="shared" si="4"/>
@@ -8160,7 +8157,7 @@
         <v>58</v>
       </c>
       <c r="S59" s="3" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="T59" s="8"/>
     </row>
@@ -8208,7 +8205,7 @@
         <v>142</v>
       </c>
       <c r="O60" s="3" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="P60" t="str">
         <f t="shared" si="4"/>
@@ -8222,7 +8219,7 @@
         <v>59</v>
       </c>
       <c r="S60" s="3" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="T60" s="8"/>
     </row>
@@ -8284,7 +8281,7 @@
         <v>60</v>
       </c>
       <c r="S61" s="3" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="T61" s="8"/>
     </row>
@@ -8346,7 +8343,7 @@
         <v>61</v>
       </c>
       <c r="S62" s="3" t="s">
-        <v>1075</v>
+        <v>1072</v>
       </c>
       <c r="T62" s="8"/>
     </row>
@@ -8408,7 +8405,7 @@
         <v>62</v>
       </c>
       <c r="S63" s="3" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="T63" s="8"/>
     </row>
@@ -8456,7 +8453,7 @@
         <v>221</v>
       </c>
       <c r="O64" s="3" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="P64" t="str">
         <f t="shared" si="4"/>
@@ -8470,7 +8467,7 @@
         <v>63</v>
       </c>
       <c r="S64" s="3" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="T64" s="8"/>
     </row>
@@ -8518,7 +8515,7 @@
         <v>508</v>
       </c>
       <c r="O65" s="3" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="P65" t="str">
         <f t="shared" si="4"/>
@@ -8532,7 +8529,7 @@
         <v>64</v>
       </c>
       <c r="S65" s="3" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="T65" s="8"/>
     </row>
@@ -8580,7 +8577,7 @@
         <v>200</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="P66" t="str">
         <f t="shared" si="4"/>
@@ -8594,7 +8591,7 @@
         <v>65</v>
       </c>
       <c r="S66" s="3" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="T66" s="8"/>
     </row>
@@ -8642,7 +8639,7 @@
         <v>49</v>
       </c>
       <c r="O67" s="3" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="P67" t="str">
         <f t="shared" si="4"/>
@@ -8656,7 +8653,7 @@
         <v>66</v>
       </c>
       <c r="S67" s="3" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="T67" s="8"/>
     </row>
@@ -8704,7 +8701,7 @@
         <v>500</v>
       </c>
       <c r="O68" s="3" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="P68" t="str">
         <f t="shared" si="4"/>
@@ -8718,7 +8715,7 @@
         <v>67</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="T68" s="8"/>
     </row>
@@ -8780,7 +8777,7 @@
         <v>68</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="T69" s="8"/>
     </row>
@@ -8842,7 +8839,7 @@
         <v>69</v>
       </c>
       <c r="S70" s="3" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="T70" s="8"/>
     </row>
@@ -8890,7 +8887,7 @@
         <v>295</v>
       </c>
       <c r="O71" s="3" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="P71" t="str">
         <f t="shared" si="6"/>
@@ -8904,7 +8901,7 @@
         <v>70</v>
       </c>
       <c r="S71" s="3" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="T71" s="8"/>
     </row>
@@ -8952,7 +8949,7 @@
         <v>328</v>
       </c>
       <c r="O72" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="P72" t="str">
         <f t="shared" si="6"/>
@@ -8966,7 +8963,7 @@
         <v>71</v>
       </c>
       <c r="S72" s="3" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="T72" s="8"/>
     </row>
@@ -9014,7 +9011,7 @@
         <v>321</v>
       </c>
       <c r="O73" s="3" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="P73" t="str">
         <f t="shared" si="6"/>
@@ -9028,7 +9025,7 @@
         <v>72</v>
       </c>
       <c r="S73" s="3" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="T73" s="8"/>
     </row>
@@ -9090,7 +9087,7 @@
         <v>73</v>
       </c>
       <c r="S74" s="3" t="s">
-        <v>1076</v>
+        <v>1073</v>
       </c>
       <c r="T74" s="8"/>
     </row>
@@ -9138,7 +9135,7 @@
         <v>667</v>
       </c>
       <c r="O75" s="3" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="P75" t="str">
         <f t="shared" si="6"/>
@@ -9152,7 +9149,7 @@
         <v>74</v>
       </c>
       <c r="S75" s="3" t="s">
-        <v>1077</v>
+        <v>1074</v>
       </c>
       <c r="T75" s="8"/>
     </row>
@@ -9200,7 +9197,7 @@
         <v>345</v>
       </c>
       <c r="O76" s="3" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="P76" t="str">
         <f t="shared" si="6"/>
@@ -9214,7 +9211,7 @@
         <v>75</v>
       </c>
       <c r="S76" s="3" t="s">
-        <v>1078</v>
+        <v>1075</v>
       </c>
       <c r="T76" s="8"/>
     </row>
@@ -9276,7 +9273,7 @@
         <v>76</v>
       </c>
       <c r="S77" s="3" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="T77" s="8"/>
     </row>
@@ -9324,7 +9321,7 @@
         <v>104</v>
       </c>
       <c r="O78" s="3" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="P78" t="str">
         <f t="shared" si="6"/>
@@ -9338,7 +9335,7 @@
         <v>77</v>
       </c>
       <c r="S78" s="3" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="T78" s="8"/>
     </row>
@@ -9400,7 +9397,7 @@
         <v>78</v>
       </c>
       <c r="S79" s="3" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="T79" s="8"/>
     </row>
@@ -9448,7 +9445,7 @@
         <v>161</v>
       </c>
       <c r="O80" s="3" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="P80" t="str">
         <f t="shared" ref="P80:P99" si="8">IF(COUNTIF(S80,"*adj*")&gt;0,"+","-")</f>
@@ -9462,7 +9459,7 @@
         <v>79</v>
       </c>
       <c r="S80" s="3" t="s">
-        <v>1081</v>
+        <v>1078</v>
       </c>
       <c r="T80" s="8"/>
     </row>
@@ -9524,7 +9521,7 @@
         <v>80</v>
       </c>
       <c r="S81" s="3" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="T81" s="8"/>
     </row>
@@ -9572,7 +9569,7 @@
         <v>396</v>
       </c>
       <c r="O82" s="3" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="P82" t="str">
         <f>IF(COUNTIF(S82,"*adj*")&gt;0,"+","-")</f>
@@ -9586,7 +9583,7 @@
         <v>81</v>
       </c>
       <c r="S82" s="3" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="T82" s="8"/>
     </row>
@@ -9634,7 +9631,7 @@
         <v>121</v>
       </c>
       <c r="O83" s="3" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="P83" t="str">
         <f t="shared" si="8"/>
@@ -9648,7 +9645,7 @@
         <v>82</v>
       </c>
       <c r="S83" s="3" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="T83" s="8"/>
     </row>
@@ -9696,7 +9693,7 @@
         <v>392</v>
       </c>
       <c r="O84" s="3" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="P84" t="str">
         <f t="shared" si="8"/>
@@ -9710,7 +9707,7 @@
         <v>83</v>
       </c>
       <c r="S84" s="3" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
       <c r="T84" s="8"/>
     </row>
@@ -9758,7 +9755,7 @@
         <v>545</v>
       </c>
       <c r="O85" s="3" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="P85" t="str">
         <f t="shared" si="8"/>
@@ -9772,7 +9769,7 @@
         <v>84</v>
       </c>
       <c r="S85" s="3" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="T85" s="8"/>
     </row>
@@ -9834,7 +9831,7 @@
         <v>85</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="T86" s="8"/>
     </row>
@@ -9896,7 +9893,7 @@
         <v>86</v>
       </c>
       <c r="S87" s="3" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="T87" s="8"/>
     </row>
@@ -9944,7 +9941,7 @@
         <v>631</v>
       </c>
       <c r="O88" s="3" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="P88" t="str">
         <f t="shared" si="8"/>
@@ -9958,7 +9955,7 @@
         <v>87</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="T88" s="8"/>
     </row>
@@ -10006,7 +10003,7 @@
         <v>253</v>
       </c>
       <c r="O89" s="3" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="P89" t="str">
         <f t="shared" si="8"/>
@@ -10020,7 +10017,7 @@
         <v>88</v>
       </c>
       <c r="S89" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="T89" s="8"/>
     </row>
@@ -10082,7 +10079,7 @@
         <v>89</v>
       </c>
       <c r="S90" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="T90" s="8"/>
     </row>
@@ -10144,7 +10141,7 @@
         <v>90</v>
       </c>
       <c r="S91" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="T91" s="8"/>
     </row>
@@ -10206,7 +10203,7 @@
         <v>91</v>
       </c>
       <c r="S92" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="T92" s="8"/>
     </row>
@@ -10268,7 +10265,7 @@
         <v>92</v>
       </c>
       <c r="S93" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="T93" s="8"/>
     </row>
@@ -10330,7 +10327,7 @@
         <v>93</v>
       </c>
       <c r="S94" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="T94" s="8"/>
     </row>
@@ -10378,7 +10375,7 @@
         <v>276</v>
       </c>
       <c r="O95" s="3" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="P95" t="str">
         <f t="shared" si="8"/>
@@ -10392,7 +10389,7 @@
         <v>94</v>
       </c>
       <c r="S95" s="3" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="T95" s="8"/>
     </row>
@@ -10440,7 +10437,7 @@
         <v>177</v>
       </c>
       <c r="O96" s="3" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="P96" t="str">
         <f t="shared" si="8"/>
@@ -10454,7 +10451,7 @@
         <v>95</v>
       </c>
       <c r="S96" s="3" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="T96" s="8"/>
     </row>
@@ -10502,7 +10499,7 @@
         <v>168</v>
       </c>
       <c r="O97" s="3" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="P97" t="str">
         <f t="shared" si="8"/>
@@ -10516,7 +10513,7 @@
         <v>96</v>
       </c>
       <c r="S97" s="3" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="T97" s="8"/>
     </row>
@@ -10564,7 +10561,7 @@
         <v>358</v>
       </c>
       <c r="O98" s="3" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="P98" t="str">
         <f t="shared" si="8"/>
@@ -10578,7 +10575,7 @@
         <v>97</v>
       </c>
       <c r="S98" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="T98" s="8"/>
     </row>
@@ -10640,7 +10637,7 @@
         <v>98</v>
       </c>
       <c r="S99" s="3" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="T99" s="8"/>
     </row>
@@ -10702,7 +10699,7 @@
         <v>99</v>
       </c>
       <c r="S100" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="T100" s="8"/>
     </row>
@@ -10750,7 +10747,7 @@
         <v>158</v>
       </c>
       <c r="O101" s="3" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="P101" t="str">
         <f t="shared" si="10"/>
@@ -10764,7 +10761,7 @@
         <v>100</v>
       </c>
       <c r="S101" s="3" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="T101" s="8"/>
     </row>
@@ -10812,7 +10809,7 @@
         <v>204</v>
       </c>
       <c r="O102" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="P102" t="str">
         <f t="shared" ref="P102:P130" si="12">IF(COUNTIF(S102,"*adj*")&gt;0,"+","-")</f>
@@ -10826,7 +10823,7 @@
         <v>101</v>
       </c>
       <c r="S102" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="T102" s="8"/>
     </row>
@@ -10888,7 +10885,7 @@
         <v>102</v>
       </c>
       <c r="S103" s="3" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="T103" s="8"/>
     </row>
@@ -10936,7 +10933,7 @@
         <v>363</v>
       </c>
       <c r="O104" s="3" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="P104" t="str">
         <f t="shared" si="12"/>
@@ -10950,7 +10947,7 @@
         <v>103</v>
       </c>
       <c r="S104" s="3" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="T104" s="8"/>
     </row>
@@ -10998,7 +10995,7 @@
         <v>287</v>
       </c>
       <c r="O105" s="3" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="P105" t="str">
         <f t="shared" si="12"/>
@@ -11012,7 +11009,7 @@
         <v>104</v>
       </c>
       <c r="S105" s="3" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="T105" s="8"/>
     </row>
@@ -11074,7 +11071,7 @@
         <v>105</v>
       </c>
       <c r="S106" s="3" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="T106" s="8"/>
     </row>
@@ -11136,7 +11133,7 @@
         <v>106</v>
       </c>
       <c r="S107" s="3" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="T107" s="8"/>
     </row>
@@ -11184,7 +11181,7 @@
         <v>87</v>
       </c>
       <c r="O108" s="3" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="P108" t="str">
         <f t="shared" si="12"/>
@@ -11198,7 +11195,7 @@
         <v>107</v>
       </c>
       <c r="S108" s="3" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="T108" s="8"/>
     </row>
@@ -11246,7 +11243,7 @@
         <v>96</v>
       </c>
       <c r="O109" s="3" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="P109" t="str">
         <f t="shared" si="12"/>
@@ -11260,7 +11257,7 @@
         <v>108</v>
       </c>
       <c r="S109" s="3" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="T109" s="8"/>
     </row>
@@ -11322,11 +11319,11 @@
         <v>109</v>
       </c>
       <c r="S110" s="3" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="T110" s="8"/>
       <c r="U110" t="s">
-        <v>1088</v>
+        <v>1084</v>
       </c>
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.25">
@@ -11373,7 +11370,7 @@
         <v>680</v>
       </c>
       <c r="O111" s="3" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="P111" t="str">
         <f t="shared" si="12"/>
@@ -11387,7 +11384,7 @@
         <v>110</v>
       </c>
       <c r="S111" s="3" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="T111" s="8"/>
     </row>
@@ -11435,7 +11432,7 @@
         <v>189</v>
       </c>
       <c r="O112" s="3" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="P112" t="str">
         <f t="shared" si="12"/>
@@ -11449,7 +11446,7 @@
         <v>111</v>
       </c>
       <c r="S112" s="3" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="T112" s="8"/>
     </row>
@@ -11511,7 +11508,7 @@
         <v>112</v>
       </c>
       <c r="S113" s="3" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="T113" s="8"/>
     </row>
@@ -11559,7 +11556,7 @@
         <v>117</v>
       </c>
       <c r="O114" s="3" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="P114" t="str">
         <f t="shared" si="12"/>
@@ -11573,7 +11570,7 @@
         <v>113</v>
       </c>
       <c r="S114" s="3" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="T114" s="8"/>
     </row>
@@ -11635,7 +11632,7 @@
         <v>114</v>
       </c>
       <c r="S115" s="3" t="s">
-        <v>1089</v>
+        <v>1085</v>
       </c>
       <c r="T115" s="8"/>
     </row>
@@ -11683,7 +11680,7 @@
         <v>619</v>
       </c>
       <c r="O116" s="3" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="P116" t="str">
         <f t="shared" si="12"/>
@@ -11697,7 +11694,7 @@
         <v>115</v>
       </c>
       <c r="S116" s="3" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="T116" s="8"/>
     </row>
@@ -11745,7 +11742,7 @@
         <v>722</v>
       </c>
       <c r="O117" s="3" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="P117" t="str">
         <f t="shared" si="12"/>
@@ -11759,7 +11756,7 @@
         <v>116</v>
       </c>
       <c r="S117" s="3" t="s">
-        <v>1052</v>
+        <v>1051</v>
       </c>
       <c r="T117" s="8"/>
     </row>
@@ -11807,7 +11804,7 @@
         <v>70</v>
       </c>
       <c r="O118" s="3" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="P118" t="str">
         <f t="shared" si="12"/>
@@ -11821,7 +11818,7 @@
         <v>117</v>
       </c>
       <c r="S118" s="3" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
       <c r="T118" s="8"/>
     </row>
@@ -11869,7 +11866,7 @@
         <v>341</v>
       </c>
       <c r="O119" s="3" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="P119" t="str">
         <f t="shared" si="12"/>
@@ -11883,7 +11880,7 @@
         <v>118</v>
       </c>
       <c r="S119" s="3" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="T119" s="8"/>
     </row>
@@ -11945,11 +11942,11 @@
         <v>119</v>
       </c>
       <c r="S120" s="3" t="s">
-        <v>1090</v>
+        <v>1086</v>
       </c>
       <c r="T120" s="8"/>
       <c r="U120" t="s">
-        <v>1091</v>
+        <v>1087</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.25">
@@ -11996,7 +11993,7 @@
         <v>181</v>
       </c>
       <c r="O121" s="3" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="P121" t="str">
         <f t="shared" si="12"/>
@@ -12010,7 +12007,7 @@
         <v>120</v>
       </c>
       <c r="S121" s="3" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="T121" s="8"/>
     </row>
@@ -12058,7 +12055,7 @@
         <v>204</v>
       </c>
       <c r="O122" s="3" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="P122" t="str">
         <f t="shared" si="12"/>
@@ -12072,7 +12069,7 @@
         <v>121</v>
       </c>
       <c r="S122" s="3" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="T122" s="8"/>
     </row>
@@ -12120,7 +12117,7 @@
         <v>336</v>
       </c>
       <c r="O123" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="P123" t="str">
         <f t="shared" si="12"/>
@@ -12134,7 +12131,7 @@
         <v>122</v>
       </c>
       <c r="S123" s="3" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="T123" s="8"/>
     </row>
@@ -12182,7 +12179,7 @@
         <v>476</v>
       </c>
       <c r="O124" s="3" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="P124" t="str">
         <f t="shared" si="12"/>
@@ -12196,7 +12193,7 @@
         <v>123</v>
       </c>
       <c r="S124" s="3" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="T124" s="8"/>
     </row>
@@ -12244,7 +12241,7 @@
         <v>473</v>
       </c>
       <c r="O125" s="3" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="P125" t="str">
         <f t="shared" si="12"/>
@@ -12258,7 +12255,7 @@
         <v>124</v>
       </c>
       <c r="S125" s="3" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="T125" s="8"/>
     </row>
@@ -12368,7 +12365,7 @@
         <v>196</v>
       </c>
       <c r="O127" s="3" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="P127" t="str">
         <f t="shared" si="12"/>
@@ -12382,7 +12379,7 @@
         <v>126</v>
       </c>
       <c r="S127" s="3" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="T127" s="8"/>
     </row>
@@ -12444,7 +12441,7 @@
         <v>127</v>
       </c>
       <c r="S128" s="3" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="T128" s="8"/>
     </row>
@@ -12506,7 +12503,7 @@
         <v>128</v>
       </c>
       <c r="S129" s="3" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="T129" s="8"/>
     </row>
@@ -12568,100 +12565,100 @@
         <v>129</v>
       </c>
       <c r="S130" s="3" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="T130" s="8"/>
       <c r="U130" t="s">
-        <v>1092</v>
-      </c>
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="131" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>23</v>
+      </c>
+      <c r="B131">
+        <v>110</v>
+      </c>
+      <c r="C131" t="s">
+        <v>398</v>
+      </c>
+      <c r="D131">
+        <v>196</v>
+      </c>
+      <c r="E131" s="1">
+        <v>5281</v>
+      </c>
+      <c r="F131" s="1">
+        <v>2938</v>
+      </c>
+      <c r="G131">
+        <v>3</v>
+      </c>
+      <c r="H131">
+        <v>16</v>
+      </c>
+      <c r="I131">
+        <v>16</v>
+      </c>
+      <c r="J131">
+        <v>0</v>
+      </c>
+      <c r="K131" s="1">
+        <v>2843</v>
+      </c>
+      <c r="L131" t="s">
+        <v>411</v>
+      </c>
+      <c r="M131" t="s">
+        <v>412</v>
+      </c>
+      <c r="N131" t="s">
+        <v>413</v>
+      </c>
+      <c r="O131" s="3" t="s">
+        <v>822</v>
+      </c>
+      <c r="P131" t="str">
+        <f>IF(COUNTIF(S131,"*adj*")&gt;0,"+","-")</f>
+        <v>-</v>
+      </c>
+      <c r="Q131" t="str">
+        <f>IF(COUNTIF(S131,"*word=*")&gt;0,"-","+")</f>
+        <v>+</v>
+      </c>
+      <c r="R131">
+        <v>130</v>
+      </c>
+      <c r="S131" s="3" t="s">
+        <v>1173</v>
+      </c>
+      <c r="T131" s="10"/>
     </row>
     <row r="132" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A132" s="5"/>
-      <c r="B132" s="5"/>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
-      <c r="E132" s="5"/>
-      <c r="F132" s="5"/>
-      <c r="G132" s="5"/>
-      <c r="H132" s="5"/>
-      <c r="I132" s="5"/>
-      <c r="J132" s="5"/>
-      <c r="K132" s="5"/>
-      <c r="L132" s="5"/>
-      <c r="M132" s="5"/>
-      <c r="N132" s="5"/>
-      <c r="O132" s="5"/>
-      <c r="P132" s="5"/>
-      <c r="Q132" s="5"/>
-      <c r="R132" s="5"/>
-      <c r="S132" s="5"/>
-      <c r="T132" s="5"/>
-      <c r="U132" s="5"/>
       <c r="V132" s="5"/>
     </row>
-    <row r="134" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>651</v>
-      </c>
-      <c r="B134">
-        <v>175</v>
-      </c>
-      <c r="C134" t="s">
-        <v>398</v>
-      </c>
-      <c r="D134">
-        <v>1020</v>
-      </c>
-      <c r="E134" s="1">
-        <v>6928</v>
-      </c>
-      <c r="F134" t="s">
-        <v>179</v>
-      </c>
-      <c r="G134">
-        <v>3</v>
-      </c>
-      <c r="H134">
-        <v>16</v>
-      </c>
-      <c r="I134">
-        <v>16</v>
-      </c>
-      <c r="J134">
-        <v>0</v>
-      </c>
-      <c r="K134" s="1">
-        <v>3147</v>
-      </c>
-      <c r="L134" s="1">
-        <v>1477</v>
-      </c>
-      <c r="M134" t="s">
-        <v>652</v>
-      </c>
-      <c r="N134" t="s">
-        <v>653</v>
-      </c>
-      <c r="O134" s="3" t="s">
-        <v>886</v>
-      </c>
-      <c r="P134" t="str">
-        <f>IF(COUNTIF(S134,"*adj*")&gt;0,"+","-")</f>
-        <v>+</v>
-      </c>
-      <c r="Q134" t="str">
-        <f>IF(COUNTIF(S134,"*word=*")&gt;0,"-","+")</f>
-        <v>-</v>
-      </c>
-      <c r="R134">
-        <v>130</v>
-      </c>
-      <c r="S134" s="3" t="s">
-        <v>1082</v>
-      </c>
-      <c r="T134" s="6" t="s">
-        <v>1181</v>
-      </c>
+    <row r="133" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A133" s="5"/>
+      <c r="B133" s="5"/>
+      <c r="C133" s="5"/>
+      <c r="D133" s="5"/>
+      <c r="E133" s="5"/>
+      <c r="F133" s="5"/>
+      <c r="G133" s="5"/>
+      <c r="H133" s="5"/>
+      <c r="I133" s="5"/>
+      <c r="J133" s="5"/>
+      <c r="K133" s="5"/>
+      <c r="L133" s="5"/>
+      <c r="M133" s="5"/>
+      <c r="N133" s="5"/>
+      <c r="O133" s="5"/>
+      <c r="P133" s="5"/>
+      <c r="Q133" s="5"/>
+      <c r="R133" s="5"/>
+      <c r="S133" s="5"/>
+      <c r="T133" s="5"/>
+      <c r="U133" s="5"/>
     </row>
     <row r="135" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
@@ -12707,7 +12704,7 @@
         <v>462</v>
       </c>
       <c r="O135" s="3" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="P135" t="str">
         <f>IF(COUNTIF(S135,"*adj*")&gt;0,"+","-")</f>
@@ -12721,16 +12718,14 @@
         <v>131</v>
       </c>
       <c r="S135" s="3" t="s">
-        <v>1156</v>
+        <v>1152</v>
       </c>
       <c r="T135" t="s">
-        <v>1072</v>
-      </c>
-      <c r="U135" s="6" t="s">
-        <v>1064</v>
-      </c>
+        <v>1069</v>
+      </c>
+      <c r="U135" s="6"/>
       <c r="V135" t="s">
-        <v>1073</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="136" spans="1:22" x14ac:dyDescent="0.25">
@@ -12794,11 +12789,9 @@
         <v>746</v>
       </c>
       <c r="T136" t="s">
-        <v>1098</v>
-      </c>
-      <c r="U136" s="6" t="s">
-        <v>1065</v>
-      </c>
+        <v>1094</v>
+      </c>
+      <c r="U136" s="6"/>
       <c r="V136" t="s">
         <v>814</v>
       </c>
@@ -12847,7 +12840,7 @@
         <v>670</v>
       </c>
       <c r="O137" s="3" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="P137" t="str">
         <f t="shared" si="14"/>
@@ -12861,13 +12854,13 @@
         <v>133</v>
       </c>
       <c r="S137" s="3" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="T137" s="6" t="s">
-        <v>1102</v>
+        <v>1098</v>
       </c>
       <c r="V137" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="138" spans="1:22" x14ac:dyDescent="0.25">
@@ -12914,7 +12907,7 @@
         <v>450</v>
       </c>
       <c r="O138" s="3" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="P138" t="str">
         <f t="shared" si="14"/>
@@ -12928,13 +12921,13 @@
         <v>134</v>
       </c>
       <c r="S138" s="3" t="s">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="T138" s="6" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
       <c r="V138" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
     </row>
     <row r="139" spans="1:22" x14ac:dyDescent="0.25">
@@ -12995,10 +12988,10 @@
         <v>135</v>
       </c>
       <c r="S139" s="3" t="s">
-        <v>1057</v>
+        <v>1056</v>
       </c>
       <c r="T139" s="6" t="s">
-        <v>1103</v>
+        <v>1099</v>
       </c>
       <c r="V139" t="s">
         <v>803</v>
@@ -13048,7 +13041,7 @@
         <v>530</v>
       </c>
       <c r="O140" s="3" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="P140" t="str">
         <f t="shared" si="14"/>
@@ -13062,13 +13055,13 @@
         <v>136</v>
       </c>
       <c r="S140" s="3" t="s">
-        <v>1157</v>
+        <v>1153</v>
       </c>
       <c r="T140" s="6" t="s">
-        <v>1112</v>
+        <v>1108</v>
       </c>
       <c r="V140" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="141" spans="1:22" x14ac:dyDescent="0.25">
@@ -13129,10 +13122,10 @@
         <v>137</v>
       </c>
       <c r="S141" s="3" t="s">
-        <v>1159</v>
+        <v>1155</v>
       </c>
       <c r="T141" s="6" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
       <c r="V141" t="s">
         <v>804</v>
@@ -13196,10 +13189,10 @@
         <v>138</v>
       </c>
       <c r="S142" s="3" t="s">
-        <v>1059</v>
+        <v>1058</v>
       </c>
       <c r="T142" s="6" t="s">
-        <v>1104</v>
+        <v>1100</v>
       </c>
       <c r="V142" t="s">
         <v>800</v>
@@ -13249,7 +13242,7 @@
         <v>479</v>
       </c>
       <c r="O143" s="3" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="P143" t="str">
         <f t="shared" si="14"/>
@@ -13263,13 +13256,13 @@
         <v>139</v>
       </c>
       <c r="S143" s="3" t="s">
-        <v>1158</v>
+        <v>1154</v>
       </c>
       <c r="T143" s="6" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
       <c r="V143" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="144" spans="1:22" x14ac:dyDescent="0.25">
@@ -13330,10 +13323,10 @@
         <v>140</v>
       </c>
       <c r="S144" s="3" t="s">
-        <v>1160</v>
+        <v>1156</v>
       </c>
       <c r="T144" s="6" t="s">
-        <v>1105</v>
+        <v>1101</v>
       </c>
       <c r="V144" t="s">
         <v>802</v>
@@ -13383,7 +13376,7 @@
         <v>586</v>
       </c>
       <c r="O145" s="3" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="P145" t="str">
         <f t="shared" si="14"/>
@@ -13397,13 +13390,13 @@
         <v>141</v>
       </c>
       <c r="S145" s="3" t="s">
-        <v>1060</v>
+        <v>1059</v>
       </c>
       <c r="T145" s="7" t="s">
-        <v>1106</v>
+        <v>1102</v>
       </c>
       <c r="V145" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="146" spans="1:22" x14ac:dyDescent="0.25">
@@ -13450,7 +13443,7 @@
         <v>616</v>
       </c>
       <c r="O146" s="3" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="P146" t="str">
         <f t="shared" si="14"/>
@@ -13464,13 +13457,13 @@
         <v>142</v>
       </c>
       <c r="S146" s="3" t="s">
-        <v>1061</v>
+        <v>1060</v>
       </c>
       <c r="T146" s="7" t="s">
-        <v>1107</v>
+        <v>1103</v>
       </c>
       <c r="V146" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="147" spans="1:22" x14ac:dyDescent="0.25">
@@ -13531,10 +13524,10 @@
         <v>143</v>
       </c>
       <c r="S147" s="3" t="s">
-        <v>1062</v>
+        <v>1061</v>
       </c>
       <c r="T147" s="7" t="s">
-        <v>1095</v>
+        <v>1091</v>
       </c>
       <c r="V147" t="s">
         <v>805</v>
@@ -13598,13 +13591,13 @@
         <v>144</v>
       </c>
       <c r="S148" s="3" t="s">
-        <v>1094</v>
+        <v>1090</v>
       </c>
       <c r="T148" s="7" t="s">
-        <v>1100</v>
+        <v>1096</v>
       </c>
       <c r="V148" t="s">
-        <v>1093</v>
+        <v>1089</v>
       </c>
     </row>
     <row r="149" spans="1:22" x14ac:dyDescent="0.25">
@@ -13623,10 +13616,10 @@
         <v>145</v>
       </c>
       <c r="S149" s="3" t="s">
-        <v>1117</v>
+        <v>1113</v>
       </c>
       <c r="T149" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="V149" t="s">
         <v>820</v>
@@ -13690,10 +13683,10 @@
         <v>146</v>
       </c>
       <c r="S150" s="3" t="s">
-        <v>1118</v>
+        <v>1114</v>
       </c>
       <c r="T150" t="s">
-        <v>1108</v>
+        <v>1104</v>
       </c>
       <c r="V150" t="s">
         <v>821</v>
@@ -13743,7 +13736,7 @@
         <v>719</v>
       </c>
       <c r="O151" s="3" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="P151" t="str">
         <f t="shared" si="16"/>
@@ -13757,13 +13750,13 @@
         <v>147</v>
       </c>
       <c r="S151" s="3" t="s">
-        <v>1161</v>
+        <v>1157</v>
       </c>
       <c r="T151" t="s">
-        <v>1096</v>
+        <v>1092</v>
       </c>
       <c r="V151" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="152" spans="1:22" x14ac:dyDescent="0.25">
@@ -13810,7 +13803,7 @@
         <v>541</v>
       </c>
       <c r="O152" s="3" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="P152" t="str">
         <f t="shared" si="16"/>
@@ -13824,13 +13817,13 @@
         <v>148</v>
       </c>
       <c r="S152" s="3" t="s">
-        <v>1124</v>
+        <v>1120</v>
       </c>
       <c r="T152" t="s">
-        <v>1109</v>
+        <v>1105</v>
       </c>
       <c r="V152" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="153" spans="1:22" x14ac:dyDescent="0.25">
@@ -13877,7 +13870,7 @@
         <v>664</v>
       </c>
       <c r="O153" s="3" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="P153" t="str">
         <f t="shared" si="16"/>
@@ -13891,13 +13884,13 @@
         <v>149</v>
       </c>
       <c r="S153" s="3" t="s">
-        <v>1162</v>
+        <v>1158</v>
       </c>
       <c r="T153" t="s">
-        <v>1097</v>
+        <v>1093</v>
       </c>
       <c r="V153" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="154" spans="1:22" x14ac:dyDescent="0.25">
@@ -13944,7 +13937,7 @@
         <v>469</v>
       </c>
       <c r="O154" s="3" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="P154" t="str">
         <f t="shared" si="16"/>
@@ -13958,13 +13951,13 @@
         <v>150</v>
       </c>
       <c r="S154" s="3" t="s">
-        <v>1126</v>
+        <v>1122</v>
       </c>
       <c r="T154" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="V154" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="155" spans="1:22" x14ac:dyDescent="0.25">
@@ -14025,10 +14018,10 @@
         <v>151</v>
       </c>
       <c r="S155" s="3" t="s">
-        <v>1127</v>
+        <v>1123</v>
       </c>
       <c r="T155" t="s">
-        <v>1128</v>
+        <v>1124</v>
       </c>
       <c r="V155" t="s">
         <v>823</v>
@@ -14092,10 +14085,10 @@
         <v>152</v>
       </c>
       <c r="S156" s="3" t="s">
-        <v>1129</v>
+        <v>1125</v>
       </c>
       <c r="T156" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
       <c r="V156" t="s">
         <v>824</v>
@@ -14145,7 +14138,7 @@
         <v>496</v>
       </c>
       <c r="O157" s="3" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="P157" t="str">
         <f t="shared" si="14"/>
@@ -14159,13 +14152,13 @@
         <v>153</v>
       </c>
       <c r="S157" s="3" t="s">
-        <v>1130</v>
+        <v>1126</v>
       </c>
       <c r="T157" t="s">
-        <v>1110</v>
+        <v>1106</v>
       </c>
       <c r="V157" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="158" spans="1:22" x14ac:dyDescent="0.25">
@@ -14226,10 +14219,10 @@
         <v>154</v>
       </c>
       <c r="S158" s="3" t="s">
-        <v>1163</v>
+        <v>1159</v>
       </c>
       <c r="T158" t="s">
-        <v>1131</v>
+        <v>1127</v>
       </c>
       <c r="V158" t="s">
         <v>825</v>
@@ -14279,7 +14272,7 @@
         <v>695</v>
       </c>
       <c r="O159" s="3" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="P159" t="str">
         <f t="shared" si="14"/>
@@ -14293,13 +14286,13 @@
         <v>155</v>
       </c>
       <c r="S159" s="3" t="s">
-        <v>1132</v>
+        <v>1128</v>
       </c>
       <c r="T159" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="V159" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="160" spans="1:22" x14ac:dyDescent="0.25">
@@ -14360,10 +14353,10 @@
         <v>156</v>
       </c>
       <c r="S160" s="3" t="s">
-        <v>1133</v>
+        <v>1129</v>
       </c>
       <c r="T160" t="s">
-        <v>1111</v>
+        <v>1107</v>
       </c>
       <c r="V160" t="s">
         <v>810</v>
@@ -14427,10 +14420,10 @@
         <v>157</v>
       </c>
       <c r="S161" s="3" t="s">
-        <v>1135</v>
+        <v>1131</v>
       </c>
       <c r="T161" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="V161" t="s">
         <v>806</v>
@@ -14494,10 +14487,10 @@
         <v>158</v>
       </c>
       <c r="S162" s="3" t="s">
-        <v>1136</v>
+        <v>1132</v>
       </c>
       <c r="T162" t="s">
-        <v>1119</v>
+        <v>1115</v>
       </c>
       <c r="V162" t="s">
         <v>801</v>
@@ -14561,10 +14554,10 @@
         <v>159</v>
       </c>
       <c r="S163" s="3" t="s">
-        <v>1137</v>
+        <v>1133</v>
       </c>
       <c r="T163" t="s">
-        <v>1120</v>
+        <v>1116</v>
       </c>
       <c r="V163" t="s">
         <v>807</v>
@@ -14628,13 +14621,13 @@
         <v>160</v>
       </c>
       <c r="S164" s="3" t="s">
-        <v>1138</v>
+        <v>1134</v>
       </c>
       <c r="T164" t="s">
-        <v>1121</v>
+        <v>1117</v>
       </c>
       <c r="V164" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="165" spans="1:22" x14ac:dyDescent="0.25">
@@ -14695,10 +14688,10 @@
         <v>161</v>
       </c>
       <c r="S165" s="3" t="s">
-        <v>1164</v>
+        <v>1160</v>
       </c>
       <c r="T165" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
       <c r="V165" t="s">
         <v>811</v>
@@ -14762,10 +14755,10 @@
         <v>162</v>
       </c>
       <c r="S166" s="3" t="s">
-        <v>1139</v>
+        <v>1135</v>
       </c>
       <c r="T166" t="s">
-        <v>1140</v>
+        <v>1136</v>
       </c>
       <c r="V166" t="s">
         <v>812</v>
@@ -14829,10 +14822,10 @@
         <v>163</v>
       </c>
       <c r="S167" s="3" t="s">
-        <v>1141</v>
+        <v>1137</v>
       </c>
       <c r="T167" t="s">
-        <v>1123</v>
+        <v>1119</v>
       </c>
       <c r="V167" t="s">
         <v>813</v>
@@ -14882,7 +14875,7 @@
         <v>511</v>
       </c>
       <c r="O168" s="3" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="P168" t="str">
         <f t="shared" si="14"/>
@@ -14896,13 +14889,13 @@
         <v>164</v>
       </c>
       <c r="S168" s="3" t="s">
-        <v>1142</v>
+        <v>1138</v>
       </c>
       <c r="T168" t="s">
-        <v>1143</v>
+        <v>1139</v>
       </c>
       <c r="V168" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="169" spans="1:22" x14ac:dyDescent="0.25">
@@ -14963,10 +14956,10 @@
         <v>165</v>
       </c>
       <c r="S169" s="3" t="s">
-        <v>1144</v>
+        <v>1140</v>
       </c>
       <c r="T169" t="s">
-        <v>1101</v>
+        <v>1097</v>
       </c>
       <c r="V169" t="s">
         <v>809</v>
@@ -15016,7 +15009,7 @@
         <v>576</v>
       </c>
       <c r="O170" s="3" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="P170" t="str">
         <f t="shared" si="14"/>
@@ -15030,10 +15023,10 @@
         <v>166</v>
       </c>
       <c r="S170" s="3" t="s">
-        <v>1146</v>
+        <v>1142</v>
       </c>
       <c r="T170" t="s">
-        <v>1147</v>
+        <v>1143</v>
       </c>
       <c r="V170" t="s">
         <v>818</v>
@@ -15097,10 +15090,10 @@
         <v>167</v>
       </c>
       <c r="S171" s="3" t="s">
-        <v>1165</v>
+        <v>1161</v>
       </c>
       <c r="T171" t="s">
-        <v>1148</v>
+        <v>1144</v>
       </c>
       <c r="V171" t="s">
         <v>799</v>
@@ -15164,10 +15157,10 @@
         <v>168</v>
       </c>
       <c r="S172" s="3" t="s">
-        <v>1149</v>
+        <v>1145</v>
       </c>
       <c r="T172" t="s">
-        <v>1150</v>
+        <v>1146</v>
       </c>
       <c r="V172" t="s">
         <v>817</v>
@@ -15231,10 +15224,10 @@
         <v>169</v>
       </c>
       <c r="S173" s="3" t="s">
-        <v>1151</v>
+        <v>1147</v>
       </c>
       <c r="T173" t="s">
-        <v>1122</v>
+        <v>1118</v>
       </c>
     </row>
     <row r="174" spans="1:22" x14ac:dyDescent="0.25">
@@ -15281,7 +15274,7 @@
         <v>590</v>
       </c>
       <c r="O174" s="3" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="P174" t="str">
         <f t="shared" si="14"/>
@@ -15295,10 +15288,10 @@
         <v>170</v>
       </c>
       <c r="S174" s="3" t="s">
-        <v>1152</v>
+        <v>1148</v>
       </c>
       <c r="T174" t="s">
-        <v>1153</v>
+        <v>1149</v>
       </c>
       <c r="V174" t="s">
         <v>819</v>
@@ -15348,7 +15341,7 @@
         <v>443</v>
       </c>
       <c r="O175" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="P175" t="str">
         <f t="shared" ref="P175:P187" si="18">IF(COUNTIF(S175,"*adj*")&gt;0,"+","-")</f>
@@ -15362,13 +15355,13 @@
         <v>171</v>
       </c>
       <c r="S175" s="3" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="T175" t="s">
-        <v>1113</v>
+        <v>1109</v>
       </c>
       <c r="V175" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="176" spans="1:22" x14ac:dyDescent="0.25">
@@ -15415,7 +15408,7 @@
         <v>454</v>
       </c>
       <c r="O176" s="3" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="P176" t="str">
         <f t="shared" si="18"/>
@@ -15429,10 +15422,10 @@
         <v>172</v>
       </c>
       <c r="S176" s="3" t="s">
-        <v>1145</v>
+        <v>1141</v>
       </c>
       <c r="T176" t="s">
-        <v>1099</v>
+        <v>1095</v>
       </c>
     </row>
     <row r="177" spans="1:22" x14ac:dyDescent="0.25">
@@ -15479,7 +15472,7 @@
         <v>698</v>
       </c>
       <c r="O177" s="3" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="P177" t="str">
         <f t="shared" si="18"/>
@@ -15493,10 +15486,10 @@
         <v>173</v>
       </c>
       <c r="S177" s="3" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="T177" s="6" t="s">
-        <v>1114</v>
+        <v>1110</v>
       </c>
     </row>
     <row r="178" spans="1:22" x14ac:dyDescent="0.25">
@@ -15543,7 +15536,7 @@
         <v>438</v>
       </c>
       <c r="O178" s="3" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="P178" t="str">
         <f t="shared" si="18"/>
@@ -15557,10 +15550,10 @@
         <v>174</v>
       </c>
       <c r="S178" s="3" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="T178" s="6" t="s">
-        <v>1072</v>
+        <v>1069</v>
       </c>
     </row>
     <row r="179" spans="1:22" x14ac:dyDescent="0.25">
@@ -15607,7 +15600,7 @@
         <v>701</v>
       </c>
       <c r="O179" s="3" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="P179" t="str">
         <f t="shared" si="18"/>
@@ -15621,10 +15614,10 @@
         <v>175</v>
       </c>
       <c r="S179" s="3" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="T179" s="6" t="s">
-        <v>1166</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="180" spans="1:22" x14ac:dyDescent="0.25">
@@ -15671,7 +15664,7 @@
         <v>432</v>
       </c>
       <c r="O180" s="3" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="P180" t="str">
         <f t="shared" si="18"/>
@@ -15685,10 +15678,10 @@
         <v>176</v>
       </c>
       <c r="S180" s="3" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="T180" s="6" t="s">
-        <v>1166</v>
+        <v>1172</v>
       </c>
     </row>
     <row r="181" spans="1:22" x14ac:dyDescent="0.25">
@@ -15749,15 +15742,15 @@
         <v>177</v>
       </c>
       <c r="S181" s="3" t="s">
-        <v>1167</v>
+        <v>1162</v>
       </c>
       <c r="T181" s="6" t="s">
-        <v>1084</v>
+        <v>1080</v>
       </c>
     </row>
     <row r="182" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>1115</v>
+        <v>1111</v>
       </c>
       <c r="P182" t="str">
         <f t="shared" si="18"/>
@@ -15771,15 +15764,15 @@
         <v>178</v>
       </c>
       <c r="S182" s="3" t="s">
-        <v>1079</v>
+        <v>1076</v>
       </c>
       <c r="T182" t="s">
-        <v>1080</v>
+        <v>1077</v>
       </c>
     </row>
     <row r="183" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>1116</v>
+        <v>1112</v>
       </c>
       <c r="P183" t="str">
         <f t="shared" si="18"/>
@@ -15793,10 +15786,10 @@
         <v>179</v>
       </c>
       <c r="S183" s="3" t="s">
-        <v>1168</v>
+        <v>1163</v>
       </c>
       <c r="T183" t="s">
-        <v>1083</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="184" spans="1:22" x14ac:dyDescent="0.25">
@@ -15815,10 +15808,10 @@
         <v>180</v>
       </c>
       <c r="S184" s="3" t="s">
-        <v>1085</v>
+        <v>1081</v>
       </c>
       <c r="T184" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="185" spans="1:22" x14ac:dyDescent="0.25">
@@ -15865,7 +15858,7 @@
         <v>606</v>
       </c>
       <c r="O185" s="3" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="P185" t="str">
         <f t="shared" si="18"/>
@@ -15879,10 +15872,10 @@
         <v>181</v>
       </c>
       <c r="S185" s="3" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="T185" t="s">
-        <v>1086</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="186" spans="1:22" x14ac:dyDescent="0.25">
@@ -15929,7 +15922,7 @@
         <v>673</v>
       </c>
       <c r="O186" s="3" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="P186" t="str">
         <f t="shared" si="18"/>
@@ -15943,10 +15936,10 @@
         <v>182</v>
       </c>
       <c r="S186" s="3" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="T186" t="s">
-        <v>1087</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="187" spans="1:22" x14ac:dyDescent="0.25">
@@ -16007,349 +16000,338 @@
         <v>183</v>
       </c>
       <c r="S187" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="T187" t="s">
+        <v>1164</v>
+      </c>
+    </row>
+    <row r="188" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A188" t="s">
+        <v>501</v>
+      </c>
+      <c r="B188">
+        <v>161</v>
+      </c>
+      <c r="C188" t="s">
+        <v>398</v>
+      </c>
+      <c r="D188">
+        <v>524</v>
+      </c>
+      <c r="E188" s="1">
+        <v>6262</v>
+      </c>
+      <c r="F188" s="1">
+        <v>2143</v>
+      </c>
+      <c r="G188">
+        <v>2</v>
+      </c>
+      <c r="H188">
+        <v>16</v>
+      </c>
+      <c r="I188">
+        <v>7</v>
+      </c>
+      <c r="J188">
+        <v>9</v>
+      </c>
+      <c r="K188" s="1">
+        <v>2147</v>
+      </c>
+      <c r="L188" t="s">
+        <v>600</v>
+      </c>
+      <c r="M188" t="s">
+        <v>601</v>
+      </c>
+      <c r="N188" t="s">
+        <v>602</v>
+      </c>
+      <c r="O188" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="P188" t="str">
+        <f>IF(COUNTIF(S188,"*adj*")&gt;0,"+","-")</f>
+        <v>+</v>
+      </c>
+      <c r="Q188" t="str">
+        <f>IF(COUNTIF(S188,"*word=*")&gt;0,"-","+")</f>
+        <v>+</v>
+      </c>
+      <c r="R188">
+        <v>184</v>
+      </c>
+      <c r="S188" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="T188" t="s">
+        <v>1171</v>
+      </c>
+      <c r="V188" s="5"/>
+    </row>
+    <row r="189" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>651</v>
+      </c>
+      <c r="B189">
+        <v>175</v>
+      </c>
+      <c r="C189" t="s">
+        <v>398</v>
+      </c>
+      <c r="D189">
+        <v>1020</v>
+      </c>
+      <c r="E189" s="1">
+        <v>6928</v>
+      </c>
+      <c r="F189" t="s">
+        <v>179</v>
+      </c>
+      <c r="G189">
+        <v>3</v>
+      </c>
+      <c r="H189">
+        <v>16</v>
+      </c>
+      <c r="I189">
+        <v>16</v>
+      </c>
+      <c r="J189">
+        <v>0</v>
+      </c>
+      <c r="K189" s="1">
+        <v>3147</v>
+      </c>
+      <c r="L189" s="1">
+        <v>1477</v>
+      </c>
+      <c r="M189" t="s">
+        <v>652</v>
+      </c>
+      <c r="N189" t="s">
+        <v>653</v>
+      </c>
+      <c r="O189" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="P189" t="str">
+        <f>IF(COUNTIF(S189,"*adj*")&gt;0,"+","-")</f>
+        <v>+</v>
+      </c>
+      <c r="Q189" t="str">
+        <f>IF(COUNTIF(S189,"*word=*")&gt;0,"-","+")</f>
+        <v>-</v>
+      </c>
+      <c r="R189">
+        <v>185</v>
+      </c>
+      <c r="S189" s="3" t="s">
         <v>1174</v>
       </c>
-      <c r="T187" t="s">
+      <c r="T189" s="6" t="s">
         <v>1170</v>
       </c>
     </row>
-    <row r="188" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="V188" s="5"/>
-    </row>
-    <row r="189" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A189" s="5"/>
-      <c r="B189" s="5"/>
-      <c r="C189" s="5"/>
-      <c r="D189" s="5"/>
-      <c r="E189" s="5"/>
-      <c r="F189" s="5"/>
-      <c r="G189" s="5"/>
-      <c r="H189" s="5"/>
-      <c r="I189" s="5"/>
-      <c r="J189" s="5"/>
-      <c r="K189" s="5"/>
-      <c r="L189" s="5"/>
-      <c r="M189" s="5"/>
-      <c r="N189" s="5"/>
-      <c r="O189" s="5"/>
-      <c r="P189" s="5"/>
-      <c r="Q189" s="5"/>
-      <c r="R189" s="5"/>
-      <c r="S189" s="5"/>
-      <c r="T189" s="5"/>
-      <c r="U189" s="5"/>
-    </row>
-    <row r="191" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A191" t="s">
-        <v>501</v>
-      </c>
-      <c r="B191">
-        <v>161</v>
-      </c>
-      <c r="C191" t="s">
+    <row r="190" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A190" t="s">
+        <v>322</v>
+      </c>
+      <c r="B190">
+        <v>167</v>
+      </c>
+      <c r="C190" t="s">
         <v>398</v>
       </c>
-      <c r="D191">
-        <v>524</v>
-      </c>
-      <c r="E191" s="1">
-        <v>6262</v>
-      </c>
-      <c r="F191" s="1">
-        <v>2143</v>
-      </c>
-      <c r="G191">
+      <c r="D190">
+        <v>143</v>
+      </c>
+      <c r="E190" s="1">
+        <v>4966</v>
+      </c>
+      <c r="F190" s="1">
+        <v>1727</v>
+      </c>
+      <c r="G190">
         <v>2</v>
       </c>
-      <c r="H191">
-        <v>16</v>
-      </c>
-      <c r="I191">
+      <c r="H190">
+        <v>17</v>
+      </c>
+      <c r="I190">
+        <v>11</v>
+      </c>
+      <c r="J190">
+        <v>6</v>
+      </c>
+      <c r="K190" s="1">
+        <v>1814</v>
+      </c>
+      <c r="L190" t="s">
+        <v>281</v>
+      </c>
+      <c r="M190" t="s">
+        <v>621</v>
+      </c>
+      <c r="N190" t="s">
+        <v>622</v>
+      </c>
+      <c r="O190" s="3" t="s">
+        <v>788</v>
+      </c>
+      <c r="P190" t="str">
+        <f>IF(COUNTIF(S190,"*adj*")&gt;0,"+","-")</f>
+        <v>+</v>
+      </c>
+      <c r="Q190" t="str">
+        <f>IF(COUNTIF(S190,"*word=*")&gt;0,"-","+")</f>
+        <v>+</v>
+      </c>
+      <c r="R190">
+        <v>186</v>
+      </c>
+      <c r="S190" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="T190" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="192" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="A192" s="5"/>
+      <c r="B192" s="5"/>
+      <c r="C192" s="5"/>
+      <c r="D192" s="5"/>
+      <c r="E192" s="5"/>
+      <c r="F192" s="5"/>
+      <c r="G192" s="5"/>
+      <c r="H192" s="5"/>
+      <c r="I192" s="5"/>
+      <c r="J192" s="5"/>
+      <c r="K192" s="5"/>
+      <c r="L192" s="5"/>
+      <c r="M192" s="5"/>
+      <c r="N192" s="5"/>
+      <c r="O192" s="5"/>
+      <c r="P192" s="5"/>
+      <c r="Q192" s="5"/>
+      <c r="R192" s="5"/>
+      <c r="S192" s="5"/>
+      <c r="T192" s="5"/>
+      <c r="U192" s="5"/>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A194" t="s">
+        <v>410</v>
+      </c>
+      <c r="B194">
+        <v>134</v>
+      </c>
+      <c r="C194" t="s">
+        <v>398</v>
+      </c>
+      <c r="D194">
+        <v>9</v>
+      </c>
+      <c r="E194" s="1">
+        <v>2251</v>
+      </c>
+      <c r="F194" t="s">
+        <v>502</v>
+      </c>
+      <c r="G194">
+        <v>4</v>
+      </c>
+      <c r="H194">
+        <v>17</v>
+      </c>
+      <c r="I194">
+        <v>10</v>
+      </c>
+      <c r="J194">
         <v>7</v>
       </c>
-      <c r="J191">
-        <v>9</v>
-      </c>
-      <c r="K191" s="1">
-        <v>2147</v>
-      </c>
-      <c r="L191" t="s">
-        <v>600</v>
-      </c>
-      <c r="M191" t="s">
-        <v>601</v>
-      </c>
-      <c r="N191" t="s">
-        <v>602</v>
-      </c>
-      <c r="O191" s="3" t="s">
-        <v>840</v>
-      </c>
-      <c r="P191" t="str">
-        <f>IF(COUNTIF(S191,"*adj*")&gt;0,"+","-")</f>
-        <v>+</v>
-      </c>
-      <c r="Q191" t="str">
-        <f>IF(COUNTIF(S191,"*word=*")&gt;0,"-","+")</f>
-        <v>+</v>
-      </c>
-      <c r="R191">
-        <v>184</v>
-      </c>
-      <c r="S191" s="3" t="s">
-        <v>1134</v>
-      </c>
-      <c r="T191" t="s">
+      <c r="K194" s="1">
+        <v>3641</v>
+      </c>
+      <c r="L194" s="1">
+        <v>2288</v>
+      </c>
+      <c r="M194" t="s">
+        <v>503</v>
+      </c>
+      <c r="N194" t="s">
+        <v>504</v>
+      </c>
+      <c r="O194" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="P194" t="str">
+        <f>IF(COUNTIF(S194,"*adj*")&gt;0,"+","-")</f>
+        <v>+</v>
+      </c>
+      <c r="Q194" t="str">
+        <f>IF(COUNTIF(S194,"*word=*")&gt;0,"-","+")</f>
+        <v>+</v>
+      </c>
+      <c r="R194">
+        <v>187</v>
+      </c>
+      <c r="S194" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="T194" t="s">
+        <v>1167</v>
+      </c>
+      <c r="U194" t="s">
         <v>1175</v>
       </c>
-      <c r="U191" t="s">
-        <v>1178</v>
-      </c>
-    </row>
-    <row r="192" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A192" t="s">
-        <v>23</v>
-      </c>
-      <c r="B192">
-        <v>110</v>
-      </c>
-      <c r="C192" t="s">
-        <v>398</v>
-      </c>
-      <c r="D192">
-        <v>196</v>
-      </c>
-      <c r="E192" s="1">
-        <v>5281</v>
-      </c>
-      <c r="F192" s="1">
-        <v>2938</v>
-      </c>
-      <c r="G192">
-        <v>3</v>
-      </c>
-      <c r="H192">
-        <v>16</v>
-      </c>
-      <c r="I192">
-        <v>16</v>
-      </c>
-      <c r="J192">
-        <v>0</v>
-      </c>
-      <c r="K192" s="1">
-        <v>2843</v>
-      </c>
-      <c r="L192" t="s">
-        <v>411</v>
-      </c>
-      <c r="M192" t="s">
-        <v>412</v>
-      </c>
-      <c r="N192" t="s">
-        <v>413</v>
-      </c>
-      <c r="O192" s="3" t="s">
-        <v>822</v>
-      </c>
-      <c r="P192" t="str">
-        <f>IF(COUNTIF(S192,"*adj*")&gt;0,"+","-")</f>
-        <v>+</v>
-      </c>
-      <c r="Q192" t="str">
-        <f>IF(COUNTIF(S192,"*word=*")&gt;0,"-","+")</f>
-        <v>+</v>
-      </c>
-      <c r="R192">
-        <v>185</v>
-      </c>
-      <c r="S192" s="3" t="s">
-        <v>1169</v>
-      </c>
-      <c r="T192" t="s">
-        <v>1173</v>
-      </c>
-      <c r="V192" t="s">
-        <v>827</v>
-      </c>
-    </row>
-    <row r="193" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A193" t="s">
-        <v>322</v>
-      </c>
-      <c r="B193">
-        <v>167</v>
-      </c>
-      <c r="C193" t="s">
-        <v>398</v>
-      </c>
-      <c r="D193">
-        <v>143</v>
-      </c>
-      <c r="E193" s="1">
-        <v>4966</v>
-      </c>
-      <c r="F193" s="1">
-        <v>1727</v>
-      </c>
-      <c r="G193">
-        <v>2</v>
-      </c>
-      <c r="H193">
-        <v>17</v>
-      </c>
-      <c r="I193">
-        <v>11</v>
-      </c>
-      <c r="J193">
-        <v>6</v>
-      </c>
-      <c r="K193" s="1">
-        <v>1814</v>
-      </c>
-      <c r="L193" t="s">
-        <v>281</v>
-      </c>
-      <c r="M193" t="s">
-        <v>621</v>
-      </c>
-      <c r="N193" t="s">
-        <v>622</v>
-      </c>
-      <c r="O193" s="3" t="s">
-        <v>788</v>
-      </c>
-      <c r="P193" t="str">
-        <f>IF(COUNTIF(S193,"*adj*")&gt;0,"+","-")</f>
-        <v>+</v>
-      </c>
-      <c r="Q193" t="str">
-        <f>IF(COUNTIF(S193,"*word=*")&gt;0,"-","+")</f>
-        <v>+</v>
-      </c>
-      <c r="R193">
-        <v>186</v>
-      </c>
-      <c r="S193" s="3" t="s">
-        <v>1171</v>
-      </c>
-      <c r="T193" t="s">
-        <v>1172</v>
-      </c>
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A195" s="5"/>
-      <c r="B195" s="5"/>
-      <c r="C195" s="5"/>
-      <c r="D195" s="5"/>
-      <c r="E195" s="5"/>
-      <c r="F195" s="5"/>
-      <c r="G195" s="5"/>
-      <c r="H195" s="5"/>
-      <c r="I195" s="5"/>
-      <c r="J195" s="5"/>
-      <c r="K195" s="5"/>
-      <c r="L195" s="5"/>
-      <c r="M195" s="5"/>
-      <c r="N195" s="5"/>
-      <c r="O195" s="5"/>
-      <c r="P195" s="5"/>
-      <c r="Q195" s="5"/>
-      <c r="R195" s="5"/>
-      <c r="S195" s="5"/>
-      <c r="T195" s="5"/>
-      <c r="U195" s="5"/>
+      <c r="A195" t="s">
+        <v>620</v>
+      </c>
+      <c r="P195" t="str">
+        <f>IF(COUNTIF(S195,"*adj*")&gt;0,"+","-")</f>
+        <v>+</v>
+      </c>
+      <c r="Q195" t="str">
+        <f>IF(COUNTIF(S195,"*word=*")&gt;0,"-","+")</f>
+        <v>+</v>
+      </c>
+      <c r="R195">
+        <v>188</v>
+      </c>
+      <c r="S195" s="9" t="s">
+        <v>1052</v>
+      </c>
+      <c r="T195" t="s">
+        <v>1110</v>
+      </c>
+      <c r="U195" t="s">
+        <v>1175</v>
+      </c>
+    </row>
+    <row r="196" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S196" t="s">
+        <v>808</v>
+      </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>410</v>
-      </c>
-      <c r="B197">
-        <v>134</v>
-      </c>
-      <c r="C197" t="s">
-        <v>398</v>
-      </c>
-      <c r="D197">
-        <v>9</v>
-      </c>
-      <c r="E197" s="1">
-        <v>2251</v>
-      </c>
-      <c r="F197" t="s">
-        <v>502</v>
-      </c>
-      <c r="G197">
-        <v>4</v>
-      </c>
-      <c r="H197">
-        <v>17</v>
-      </c>
-      <c r="I197">
-        <v>10</v>
-      </c>
-      <c r="J197">
-        <v>7</v>
-      </c>
-      <c r="K197" s="1">
-        <v>3641</v>
-      </c>
-      <c r="L197" s="1">
-        <v>2288</v>
-      </c>
-      <c r="M197" t="s">
-        <v>503</v>
-      </c>
-      <c r="N197" t="s">
-        <v>504</v>
-      </c>
-      <c r="O197" s="3" t="s">
-        <v>826</v>
-      </c>
-      <c r="P197" t="str">
-        <f>IF(COUNTIF(S197,"*adj*")&gt;0,"+","-")</f>
-        <v>+</v>
-      </c>
-      <c r="Q197" t="str">
-        <f>IF(COUNTIF(S197,"*word=*")&gt;0,"-","+")</f>
-        <v>+</v>
-      </c>
-      <c r="R197">
-        <v>187</v>
-      </c>
-      <c r="S197" s="3" t="s">
-        <v>1125</v>
-      </c>
-      <c r="T197" t="s">
-        <v>1176</v>
-      </c>
-      <c r="U197" t="s">
-        <v>1177</v>
+      <c r="S197" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>620</v>
-      </c>
-      <c r="P198" t="str">
-        <f>IF(COUNTIF(S198,"*adj*")&gt;0,"+","-")</f>
-        <v>+</v>
-      </c>
-      <c r="Q198" t="str">
-        <f>IF(COUNTIF(S198,"*word=*")&gt;0,"-","+")</f>
-        <v>+</v>
-      </c>
-      <c r="R198">
-        <v>188</v>
-      </c>
-      <c r="S198" s="9" t="s">
-        <v>1053</v>
-      </c>
-      <c r="T198" t="s">
-        <v>1114</v>
-      </c>
-      <c r="U198" t="s">
-        <v>1177</v>
+      <c r="S198" t="s">
+        <v>808</v>
+      </c>
+    </row>
+    <row r="199" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="S199" t="s">
+        <v>808</v>
       </c>
     </row>
     <row r="200" spans="1:21" x14ac:dyDescent="0.25">
@@ -16522,35 +16504,15 @@
         <v>808</v>
       </c>
     </row>
-    <row r="234" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S234" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="235" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S235" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="236" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S236" t="s">
-        <v>808</v>
-      </c>
-    </row>
-    <row r="237" spans="19:19" x14ac:dyDescent="0.25">
-      <c r="S237" t="s">
-        <v>808</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:S237" xr:uid="{C242313F-BBF9-4E23-B5E6-D22D773B27DE}"/>
+  <autoFilter ref="A1:S233" xr:uid="{C242313F-BBF9-4E23-B5E6-D22D773B27DE}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="24" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="3" operator="containsText" id="{83D914DD-4A90-447F-8276-C0845511F922}">
+          <x14:cfRule type="containsText" priority="5" operator="containsText" id="{83D914DD-4A90-447F-8276-C0845511F922}">
             <xm:f>NOT(ISERROR(SEARCH("+",P1)))</xm:f>
             <xm:f>"+"</xm:f>
             <x14:dxf>
@@ -16561,7 +16523,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{0891F6A0-B21A-4913-B316-A3AFD902FF35}">
+          <x14:cfRule type="containsText" priority="6" operator="containsText" id="{0891F6A0-B21A-4913-B316-A3AFD902FF35}">
             <xm:f>NOT(ISERROR(SEARCH("-",P1)))</xm:f>
             <xm:f>"-"</xm:f>
             <x14:dxf>
@@ -16572,7 +16534,32 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>T1 R1 P191:Q193 P200:P1048576 P197:Q198 P134:Q187 P1:Q130</xm:sqref>
+          <xm:sqref>T1 R1 P196:P1048576 P194:Q195 P135:Q187 P189:Q190 P1:Q131</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="1" operator="containsText" id="{ECCD568F-C7AF-4257-A650-CF2B610544C5}">
+            <xm:f>NOT(ISERROR(SEARCH("+",P188)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FF00B050"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{AF374360-42E3-45D7-A123-F6EC9C0F7500}">
+            <xm:f>NOT(ISERROR(SEARCH("-",P188)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFF0000"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>P188:Q188</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
all idioms in right categories - complete
</commit_message>
<xml_diff>
--- a/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
+++ b/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\idiom_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB4B053B-1B9F-4C19-8174-9FD0949C81A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E29E86F-C3F1-4116-8773-1C5694588145}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4472,8 +4472,8 @@
   </sheetPr>
   <dimension ref="A1:V233"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S147" sqref="S147"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T166" sqref="T166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
moved 1 idiom (included verb), calculated pmi for 1 idiom (example, made script to calculate pmi and fixedness and made one table with ttr, f-score and length
</commit_message>
<xml_diff>
--- a/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
+++ b/idiom_database/idiom_database_sprenger_with_queries_and_explanation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mijn Drive\Studie informatiekunde\master\master project\project\idiom_database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73E58B3-322D-4BA2-B01A-5737E5E65255}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D218E5D3-D228-453E-8768-F4B589FEA2C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="idiom_database" sheetId="11" r:id="rId1"/>
@@ -23,19 +23,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'idiom_database - for paper 1'!$A$1:$E$233</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4380" uniqueCount="851">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4382" uniqueCount="852">
   <si>
     <t>Idiom</t>
   </si>
@@ -2588,13 +2580,16 @@
   </si>
   <si>
     <t>Literal</t>
+  </si>
+  <si>
+    <t>WEL MET VERB - aangepast in crosstables e.d.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2735,8 +2730,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2940,6 +2943,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -3125,7 +3134,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
@@ -3169,6 +3178,9 @@
     <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3214,21 +3226,7 @@
     <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="10">
     <dxf>
       <fill>
         <patternFill>
@@ -3612,10 +3610,10 @@
   <sheetPr codeName="Blad5">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S233"/>
+  <dimension ref="A1:I233"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A61" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G76" sqref="G76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5197,23 +5195,29 @@
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="26" t="s">
         <v>503</v>
       </c>
-      <c r="B75" t="s">
+      <c r="B75" s="27" t="s">
         <v>504</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="27" t="s">
         <v>505</v>
       </c>
-      <c r="D75">
+      <c r="D75" s="27">
         <v>74</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="E75" s="27" t="s">
         <v>735</v>
       </c>
-      <c r="F75" s="5"/>
-      <c r="I75">
+      <c r="F75" s="27" t="s">
+        <v>765</v>
+      </c>
+      <c r="G75" s="27" t="s">
+        <v>851</v>
+      </c>
+      <c r="H75" s="25"/>
+      <c r="I75" s="25">
         <v>1</v>
       </c>
     </row>
@@ -8113,7 +8117,7 @@
   <sheetPr codeName="Blad4">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S233"/>
+  <dimension ref="A1:F233"/>
   <sheetViews>
     <sheetView topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
@@ -11770,7 +11774,7 @@
     <col min="1" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:195" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:195" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>718</v>
       </c>
@@ -12339,7 +12343,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:195" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:195" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
@@ -12908,7 +12912,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="3" spans="1:195" s="10" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:195" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>606</v>
       </c>
@@ -13477,7 +13481,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="4" spans="1:195" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:195" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
@@ -14046,7 +14050,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="5" spans="1:195" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:195" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -14615,7 +14619,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="6" spans="1:195" s="10" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:195" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>848</v>
       </c>
@@ -14835,7 +14839,7 @@
   <sheetPr codeName="Blad11"/>
   <dimension ref="A1:B1186"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1155" workbookViewId="0">
+    <sheetView topLeftCell="A1155" workbookViewId="0">
       <selection activeCell="E1171" sqref="E1171"/>
     </sheetView>
   </sheetViews>

</xml_diff>